<commit_message>
updated survival with 8/7 and 8/8 data
</commit_message>
<xml_diff>
--- a/data/survival/survival_resazurin.xlsx
+++ b/data/survival/survival_resazurin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/10K-seed-Cgigas/data/survival/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D232083D-93FC-FB4C-95AD-9E9424BB8FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65C3866-881D-9B4E-9A30-4C9A6682F415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33000" yWindow="-1460" windowWidth="30280" windowHeight="19380" xr2:uid="{FF76C7E6-3408-934E-9F62-D1FDE39EF6F8}"/>
+    <workbookView xWindow="2720" yWindow="760" windowWidth="25800" windowHeight="18880" xr2:uid="{FF76C7E6-3408-934E-9F62-D1FDE39EF6F8}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="17">
   <si>
     <t>date.resazurin</t>
   </si>
@@ -459,11 +459,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE0A6E7-C44F-C349-A3CE-3BF585EE18ED}">
-  <dimension ref="A1:K241"/>
+  <dimension ref="A1:K321"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <pane ySplit="1" topLeftCell="A280" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K300" sqref="K300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8906,6 +8906,2806 @@
       </c>
       <c r="K241">
         <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A242">
+        <v>20240807</v>
+      </c>
+      <c r="B242">
+        <v>47</v>
+      </c>
+      <c r="C242" t="s">
+        <v>2</v>
+      </c>
+      <c r="D242" t="s">
+        <v>11</v>
+      </c>
+      <c r="E242">
+        <v>1</v>
+      </c>
+      <c r="F242">
+        <v>0</v>
+      </c>
+      <c r="G242">
+        <v>0</v>
+      </c>
+      <c r="H242">
+        <v>0</v>
+      </c>
+      <c r="I242">
+        <v>0</v>
+      </c>
+      <c r="J242">
+        <v>0</v>
+      </c>
+      <c r="K242">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A243">
+        <v>20240807</v>
+      </c>
+      <c r="B243">
+        <v>47</v>
+      </c>
+      <c r="C243" t="s">
+        <v>2</v>
+      </c>
+      <c r="D243" t="s">
+        <v>11</v>
+      </c>
+      <c r="E243">
+        <v>2</v>
+      </c>
+      <c r="F243">
+        <v>0</v>
+      </c>
+      <c r="G243">
+        <v>0</v>
+      </c>
+      <c r="H243">
+        <v>0</v>
+      </c>
+      <c r="I243">
+        <v>0</v>
+      </c>
+      <c r="J243">
+        <v>0</v>
+      </c>
+      <c r="K243">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A244">
+        <v>20240807</v>
+      </c>
+      <c r="B244">
+        <v>47</v>
+      </c>
+      <c r="C244" t="s">
+        <v>2</v>
+      </c>
+      <c r="D244" t="s">
+        <v>11</v>
+      </c>
+      <c r="E244">
+        <v>3</v>
+      </c>
+      <c r="F244">
+        <v>0</v>
+      </c>
+      <c r="G244">
+        <v>0</v>
+      </c>
+      <c r="H244">
+        <v>0</v>
+      </c>
+      <c r="I244">
+        <v>0</v>
+      </c>
+      <c r="J244">
+        <v>0</v>
+      </c>
+      <c r="K244">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A245">
+        <v>20240807</v>
+      </c>
+      <c r="B245">
+        <v>47</v>
+      </c>
+      <c r="C245" t="s">
+        <v>2</v>
+      </c>
+      <c r="D245" t="s">
+        <v>11</v>
+      </c>
+      <c r="E245">
+        <v>4</v>
+      </c>
+      <c r="F245">
+        <v>0</v>
+      </c>
+      <c r="G245">
+        <v>0</v>
+      </c>
+      <c r="H245">
+        <v>0</v>
+      </c>
+      <c r="I245">
+        <v>0</v>
+      </c>
+      <c r="J245">
+        <v>0</v>
+      </c>
+      <c r="K245">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A246">
+        <v>20240807</v>
+      </c>
+      <c r="B246">
+        <v>47</v>
+      </c>
+      <c r="C246" t="s">
+        <v>2</v>
+      </c>
+      <c r="D246" t="s">
+        <v>11</v>
+      </c>
+      <c r="E246">
+        <v>5</v>
+      </c>
+      <c r="F246">
+        <v>0</v>
+      </c>
+      <c r="G246">
+        <v>0</v>
+      </c>
+      <c r="H246">
+        <v>0</v>
+      </c>
+      <c r="I246">
+        <v>0</v>
+      </c>
+      <c r="J246">
+        <v>0</v>
+      </c>
+      <c r="K246">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A247">
+        <v>20240807</v>
+      </c>
+      <c r="B247">
+        <v>47</v>
+      </c>
+      <c r="C247" t="s">
+        <v>2</v>
+      </c>
+      <c r="D247" t="s">
+        <v>11</v>
+      </c>
+      <c r="E247">
+        <v>6</v>
+      </c>
+      <c r="F247">
+        <v>0</v>
+      </c>
+      <c r="G247">
+        <v>0</v>
+      </c>
+      <c r="H247">
+        <v>0</v>
+      </c>
+      <c r="I247">
+        <v>0</v>
+      </c>
+      <c r="J247">
+        <v>0</v>
+      </c>
+      <c r="K247">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A248">
+        <v>20240807</v>
+      </c>
+      <c r="B248">
+        <v>47</v>
+      </c>
+      <c r="C248" t="s">
+        <v>2</v>
+      </c>
+      <c r="D248" t="s">
+        <v>11</v>
+      </c>
+      <c r="E248">
+        <v>7</v>
+      </c>
+      <c r="F248">
+        <v>0</v>
+      </c>
+      <c r="G248">
+        <v>0</v>
+      </c>
+      <c r="H248">
+        <v>0</v>
+      </c>
+      <c r="I248">
+        <v>0</v>
+      </c>
+      <c r="J248">
+        <v>0</v>
+      </c>
+      <c r="K248">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A249">
+        <v>20240807</v>
+      </c>
+      <c r="B249">
+        <v>47</v>
+      </c>
+      <c r="C249" t="s">
+        <v>2</v>
+      </c>
+      <c r="D249" t="s">
+        <v>11</v>
+      </c>
+      <c r="E249">
+        <v>8</v>
+      </c>
+      <c r="F249">
+        <v>0</v>
+      </c>
+      <c r="G249">
+        <v>0</v>
+      </c>
+      <c r="H249">
+        <v>0</v>
+      </c>
+      <c r="I249">
+        <v>0</v>
+      </c>
+      <c r="J249">
+        <v>0</v>
+      </c>
+      <c r="K249">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A250">
+        <v>20240807</v>
+      </c>
+      <c r="B250">
+        <v>47</v>
+      </c>
+      <c r="C250" t="s">
+        <v>2</v>
+      </c>
+      <c r="D250" t="s">
+        <v>11</v>
+      </c>
+      <c r="E250">
+        <v>9</v>
+      </c>
+      <c r="F250">
+        <v>0</v>
+      </c>
+      <c r="G250">
+        <v>0</v>
+      </c>
+      <c r="H250">
+        <v>0</v>
+      </c>
+      <c r="I250">
+        <v>0</v>
+      </c>
+      <c r="J250">
+        <v>0</v>
+      </c>
+      <c r="K250">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A251">
+        <v>20240807</v>
+      </c>
+      <c r="B251">
+        <v>47</v>
+      </c>
+      <c r="C251" t="s">
+        <v>2</v>
+      </c>
+      <c r="D251" t="s">
+        <v>11</v>
+      </c>
+      <c r="E251">
+        <v>10</v>
+      </c>
+      <c r="F251">
+        <v>0</v>
+      </c>
+      <c r="G251">
+        <v>0</v>
+      </c>
+      <c r="H251">
+        <v>0</v>
+      </c>
+      <c r="I251">
+        <v>0</v>
+      </c>
+      <c r="J251">
+        <v>0</v>
+      </c>
+      <c r="K251">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A252">
+        <v>20240807</v>
+      </c>
+      <c r="B252">
+        <v>47</v>
+      </c>
+      <c r="C252" t="s">
+        <v>2</v>
+      </c>
+      <c r="D252" t="s">
+        <v>11</v>
+      </c>
+      <c r="E252">
+        <v>11</v>
+      </c>
+      <c r="F252">
+        <v>0</v>
+      </c>
+      <c r="G252">
+        <v>0</v>
+      </c>
+      <c r="H252">
+        <v>0</v>
+      </c>
+      <c r="I252">
+        <v>0</v>
+      </c>
+      <c r="J252">
+        <v>0</v>
+      </c>
+      <c r="K252">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A253">
+        <v>20240807</v>
+      </c>
+      <c r="B253">
+        <v>47</v>
+      </c>
+      <c r="C253" t="s">
+        <v>2</v>
+      </c>
+      <c r="D253" t="s">
+        <v>11</v>
+      </c>
+      <c r="E253">
+        <v>12</v>
+      </c>
+      <c r="F253">
+        <v>0</v>
+      </c>
+      <c r="G253">
+        <v>0</v>
+      </c>
+      <c r="H253">
+        <v>0</v>
+      </c>
+      <c r="I253">
+        <v>0</v>
+      </c>
+      <c r="J253">
+        <v>0</v>
+      </c>
+      <c r="K253">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A254">
+        <v>20240807</v>
+      </c>
+      <c r="B254">
+        <v>47</v>
+      </c>
+      <c r="C254" t="s">
+        <v>2</v>
+      </c>
+      <c r="D254" t="s">
+        <v>11</v>
+      </c>
+      <c r="E254">
+        <v>13</v>
+      </c>
+      <c r="F254">
+        <v>0</v>
+      </c>
+      <c r="G254">
+        <v>0</v>
+      </c>
+      <c r="H254">
+        <v>0</v>
+      </c>
+      <c r="I254">
+        <v>0</v>
+      </c>
+      <c r="J254">
+        <v>0</v>
+      </c>
+      <c r="K254">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A255">
+        <v>20240807</v>
+      </c>
+      <c r="B255">
+        <v>47</v>
+      </c>
+      <c r="C255" t="s">
+        <v>2</v>
+      </c>
+      <c r="D255" t="s">
+        <v>11</v>
+      </c>
+      <c r="E255">
+        <v>14</v>
+      </c>
+      <c r="F255">
+        <v>0</v>
+      </c>
+      <c r="G255">
+        <v>0</v>
+      </c>
+      <c r="H255">
+        <v>0</v>
+      </c>
+      <c r="I255">
+        <v>0</v>
+      </c>
+      <c r="J255">
+        <v>0</v>
+      </c>
+      <c r="K255">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A256">
+        <v>20240807</v>
+      </c>
+      <c r="B256">
+        <v>47</v>
+      </c>
+      <c r="C256" t="s">
+        <v>2</v>
+      </c>
+      <c r="D256" t="s">
+        <v>11</v>
+      </c>
+      <c r="E256">
+        <v>15</v>
+      </c>
+      <c r="F256">
+        <v>0</v>
+      </c>
+      <c r="G256">
+        <v>0</v>
+      </c>
+      <c r="H256">
+        <v>0</v>
+      </c>
+      <c r="I256">
+        <v>0</v>
+      </c>
+      <c r="J256">
+        <v>0</v>
+      </c>
+      <c r="K256">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A257">
+        <v>20240807</v>
+      </c>
+      <c r="B257">
+        <v>47</v>
+      </c>
+      <c r="C257" t="s">
+        <v>2</v>
+      </c>
+      <c r="D257" t="s">
+        <v>11</v>
+      </c>
+      <c r="E257">
+        <v>16</v>
+      </c>
+      <c r="F257">
+        <v>0</v>
+      </c>
+      <c r="G257">
+        <v>0</v>
+      </c>
+      <c r="H257">
+        <v>0</v>
+      </c>
+      <c r="I257">
+        <v>0</v>
+      </c>
+      <c r="J257">
+        <v>0</v>
+      </c>
+      <c r="K257">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A258">
+        <v>20240807</v>
+      </c>
+      <c r="B258">
+        <v>47</v>
+      </c>
+      <c r="C258" t="s">
+        <v>2</v>
+      </c>
+      <c r="D258" t="s">
+        <v>11</v>
+      </c>
+      <c r="E258">
+        <v>17</v>
+      </c>
+      <c r="F258">
+        <v>0</v>
+      </c>
+      <c r="G258">
+        <v>0</v>
+      </c>
+      <c r="H258">
+        <v>0</v>
+      </c>
+      <c r="I258">
+        <v>0</v>
+      </c>
+      <c r="J258">
+        <v>0</v>
+      </c>
+      <c r="K258">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A259">
+        <v>20240807</v>
+      </c>
+      <c r="B259">
+        <v>47</v>
+      </c>
+      <c r="C259" t="s">
+        <v>2</v>
+      </c>
+      <c r="D259" t="s">
+        <v>11</v>
+      </c>
+      <c r="E259">
+        <v>18</v>
+      </c>
+      <c r="F259">
+        <v>0</v>
+      </c>
+      <c r="G259">
+        <v>0</v>
+      </c>
+      <c r="H259">
+        <v>0</v>
+      </c>
+      <c r="I259">
+        <v>0</v>
+      </c>
+      <c r="J259">
+        <v>0</v>
+      </c>
+      <c r="K259">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A260">
+        <v>20240807</v>
+      </c>
+      <c r="B260">
+        <v>47</v>
+      </c>
+      <c r="C260" t="s">
+        <v>2</v>
+      </c>
+      <c r="D260" t="s">
+        <v>11</v>
+      </c>
+      <c r="E260">
+        <v>19</v>
+      </c>
+      <c r="F260">
+        <v>0</v>
+      </c>
+      <c r="G260">
+        <v>0</v>
+      </c>
+      <c r="H260">
+        <v>0</v>
+      </c>
+      <c r="I260">
+        <v>0</v>
+      </c>
+      <c r="J260">
+        <v>0</v>
+      </c>
+      <c r="K260">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A261">
+        <v>20240807</v>
+      </c>
+      <c r="B261">
+        <v>47</v>
+      </c>
+      <c r="C261" t="s">
+        <v>2</v>
+      </c>
+      <c r="D261" t="s">
+        <v>11</v>
+      </c>
+      <c r="E261">
+        <v>20</v>
+      </c>
+      <c r="F261">
+        <v>0</v>
+      </c>
+      <c r="G261">
+        <v>0</v>
+      </c>
+      <c r="H261">
+        <v>0</v>
+      </c>
+      <c r="I261">
+        <v>0</v>
+      </c>
+      <c r="J261">
+        <v>0</v>
+      </c>
+      <c r="K261">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A262">
+        <v>20240807</v>
+      </c>
+      <c r="B262">
+        <v>47</v>
+      </c>
+      <c r="C262" t="s">
+        <v>2</v>
+      </c>
+      <c r="D262" t="s">
+        <v>12</v>
+      </c>
+      <c r="E262">
+        <v>21</v>
+      </c>
+      <c r="F262">
+        <v>0</v>
+      </c>
+      <c r="G262">
+        <v>0</v>
+      </c>
+      <c r="H262">
+        <v>0</v>
+      </c>
+      <c r="I262">
+        <v>0</v>
+      </c>
+      <c r="J262">
+        <v>1</v>
+      </c>
+      <c r="K262">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A263">
+        <v>20240807</v>
+      </c>
+      <c r="B263">
+        <v>47</v>
+      </c>
+      <c r="C263" t="s">
+        <v>2</v>
+      </c>
+      <c r="D263" t="s">
+        <v>12</v>
+      </c>
+      <c r="E263">
+        <v>22</v>
+      </c>
+      <c r="F263">
+        <v>0</v>
+      </c>
+      <c r="G263">
+        <v>0</v>
+      </c>
+      <c r="H263">
+        <v>0</v>
+      </c>
+      <c r="I263">
+        <v>0</v>
+      </c>
+      <c r="J263">
+        <v>0</v>
+      </c>
+      <c r="K263">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A264">
+        <v>20240807</v>
+      </c>
+      <c r="B264">
+        <v>47</v>
+      </c>
+      <c r="C264" t="s">
+        <v>2</v>
+      </c>
+      <c r="D264" t="s">
+        <v>12</v>
+      </c>
+      <c r="E264">
+        <v>23</v>
+      </c>
+      <c r="F264">
+        <v>0</v>
+      </c>
+      <c r="G264">
+        <v>0</v>
+      </c>
+      <c r="H264">
+        <v>1</v>
+      </c>
+      <c r="I264">
+        <v>1</v>
+      </c>
+      <c r="J264">
+        <v>1</v>
+      </c>
+      <c r="K264">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A265">
+        <v>20240807</v>
+      </c>
+      <c r="B265">
+        <v>47</v>
+      </c>
+      <c r="C265" t="s">
+        <v>2</v>
+      </c>
+      <c r="D265" t="s">
+        <v>12</v>
+      </c>
+      <c r="E265">
+        <v>24</v>
+      </c>
+      <c r="F265">
+        <v>0</v>
+      </c>
+      <c r="G265">
+        <v>0</v>
+      </c>
+      <c r="H265">
+        <v>0</v>
+      </c>
+      <c r="I265">
+        <v>1</v>
+      </c>
+      <c r="J265">
+        <v>1</v>
+      </c>
+      <c r="K265">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A266">
+        <v>20240807</v>
+      </c>
+      <c r="B266">
+        <v>47</v>
+      </c>
+      <c r="C266" t="s">
+        <v>2</v>
+      </c>
+      <c r="D266" t="s">
+        <v>12</v>
+      </c>
+      <c r="E266">
+        <v>25</v>
+      </c>
+      <c r="F266">
+        <v>0</v>
+      </c>
+      <c r="G266">
+        <v>0</v>
+      </c>
+      <c r="H266">
+        <v>1</v>
+      </c>
+      <c r="I266">
+        <v>1</v>
+      </c>
+      <c r="J266">
+        <v>1</v>
+      </c>
+      <c r="K266">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A267">
+        <v>20240807</v>
+      </c>
+      <c r="B267">
+        <v>47</v>
+      </c>
+      <c r="C267" t="s">
+        <v>2</v>
+      </c>
+      <c r="D267" t="s">
+        <v>12</v>
+      </c>
+      <c r="E267">
+        <v>26</v>
+      </c>
+      <c r="F267">
+        <v>0</v>
+      </c>
+      <c r="G267">
+        <v>0</v>
+      </c>
+      <c r="H267">
+        <v>0</v>
+      </c>
+      <c r="I267">
+        <v>0</v>
+      </c>
+      <c r="J267">
+        <v>0</v>
+      </c>
+      <c r="K267">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A268">
+        <v>20240807</v>
+      </c>
+      <c r="B268">
+        <v>47</v>
+      </c>
+      <c r="C268" t="s">
+        <v>2</v>
+      </c>
+      <c r="D268" t="s">
+        <v>12</v>
+      </c>
+      <c r="E268">
+        <v>27</v>
+      </c>
+      <c r="F268">
+        <v>0</v>
+      </c>
+      <c r="G268">
+        <v>0</v>
+      </c>
+      <c r="H268">
+        <v>0</v>
+      </c>
+      <c r="I268">
+        <v>1</v>
+      </c>
+      <c r="J268">
+        <v>1</v>
+      </c>
+      <c r="K268">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A269">
+        <v>20240807</v>
+      </c>
+      <c r="B269">
+        <v>47</v>
+      </c>
+      <c r="C269" t="s">
+        <v>2</v>
+      </c>
+      <c r="D269" t="s">
+        <v>12</v>
+      </c>
+      <c r="E269">
+        <v>28</v>
+      </c>
+      <c r="F269">
+        <v>0</v>
+      </c>
+      <c r="G269">
+        <v>0</v>
+      </c>
+      <c r="H269">
+        <v>0</v>
+      </c>
+      <c r="I269">
+        <v>0</v>
+      </c>
+      <c r="J269">
+        <v>1</v>
+      </c>
+      <c r="K269">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A270">
+        <v>20240807</v>
+      </c>
+      <c r="B270">
+        <v>47</v>
+      </c>
+      <c r="C270" t="s">
+        <v>2</v>
+      </c>
+      <c r="D270" t="s">
+        <v>12</v>
+      </c>
+      <c r="E270">
+        <v>29</v>
+      </c>
+      <c r="F270">
+        <v>0</v>
+      </c>
+      <c r="G270">
+        <v>0</v>
+      </c>
+      <c r="H270">
+        <v>0</v>
+      </c>
+      <c r="I270">
+        <v>0</v>
+      </c>
+      <c r="J270">
+        <v>1</v>
+      </c>
+      <c r="K270">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A271">
+        <v>20240807</v>
+      </c>
+      <c r="B271">
+        <v>47</v>
+      </c>
+      <c r="C271" t="s">
+        <v>2</v>
+      </c>
+      <c r="D271" t="s">
+        <v>12</v>
+      </c>
+      <c r="E271">
+        <v>30</v>
+      </c>
+      <c r="F271">
+        <v>0</v>
+      </c>
+      <c r="G271">
+        <v>0</v>
+      </c>
+      <c r="H271">
+        <v>0</v>
+      </c>
+      <c r="I271">
+        <v>0</v>
+      </c>
+      <c r="J271">
+        <v>0</v>
+      </c>
+      <c r="K271">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A272">
+        <v>20240807</v>
+      </c>
+      <c r="B272">
+        <v>47</v>
+      </c>
+      <c r="C272" t="s">
+        <v>2</v>
+      </c>
+      <c r="D272" t="s">
+        <v>12</v>
+      </c>
+      <c r="E272">
+        <v>31</v>
+      </c>
+      <c r="F272">
+        <v>0</v>
+      </c>
+      <c r="G272">
+        <v>0</v>
+      </c>
+      <c r="H272">
+        <v>1</v>
+      </c>
+      <c r="I272">
+        <v>1</v>
+      </c>
+      <c r="J272">
+        <v>1</v>
+      </c>
+      <c r="K272">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A273">
+        <v>20240807</v>
+      </c>
+      <c r="B273">
+        <v>47</v>
+      </c>
+      <c r="C273" t="s">
+        <v>2</v>
+      </c>
+      <c r="D273" t="s">
+        <v>12</v>
+      </c>
+      <c r="E273">
+        <v>32</v>
+      </c>
+      <c r="F273">
+        <v>0</v>
+      </c>
+      <c r="G273">
+        <v>0</v>
+      </c>
+      <c r="H273">
+        <v>1</v>
+      </c>
+      <c r="I273">
+        <v>1</v>
+      </c>
+      <c r="J273">
+        <v>1</v>
+      </c>
+      <c r="K273">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="274" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A274">
+        <v>20240807</v>
+      </c>
+      <c r="B274">
+        <v>47</v>
+      </c>
+      <c r="C274" t="s">
+        <v>2</v>
+      </c>
+      <c r="D274" t="s">
+        <v>12</v>
+      </c>
+      <c r="E274">
+        <v>33</v>
+      </c>
+      <c r="F274">
+        <v>0</v>
+      </c>
+      <c r="G274">
+        <v>0</v>
+      </c>
+      <c r="H274">
+        <v>0</v>
+      </c>
+      <c r="I274">
+        <v>0</v>
+      </c>
+      <c r="J274">
+        <v>0</v>
+      </c>
+      <c r="K274">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A275">
+        <v>20240807</v>
+      </c>
+      <c r="B275">
+        <v>47</v>
+      </c>
+      <c r="C275" t="s">
+        <v>2</v>
+      </c>
+      <c r="D275" t="s">
+        <v>12</v>
+      </c>
+      <c r="E275">
+        <v>34</v>
+      </c>
+      <c r="F275">
+        <v>0</v>
+      </c>
+      <c r="G275">
+        <v>0</v>
+      </c>
+      <c r="H275">
+        <v>1</v>
+      </c>
+      <c r="I275">
+        <v>1</v>
+      </c>
+      <c r="J275">
+        <v>1</v>
+      </c>
+      <c r="K275">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A276">
+        <v>20240807</v>
+      </c>
+      <c r="B276">
+        <v>47</v>
+      </c>
+      <c r="C276" t="s">
+        <v>2</v>
+      </c>
+      <c r="D276" t="s">
+        <v>12</v>
+      </c>
+      <c r="E276">
+        <v>35</v>
+      </c>
+      <c r="F276">
+        <v>0</v>
+      </c>
+      <c r="G276">
+        <v>0</v>
+      </c>
+      <c r="H276">
+        <v>0</v>
+      </c>
+      <c r="I276">
+        <v>0</v>
+      </c>
+      <c r="J276">
+        <v>1</v>
+      </c>
+      <c r="K276">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A277">
+        <v>20240807</v>
+      </c>
+      <c r="B277">
+        <v>47</v>
+      </c>
+      <c r="C277" t="s">
+        <v>2</v>
+      </c>
+      <c r="D277" t="s">
+        <v>12</v>
+      </c>
+      <c r="E277">
+        <v>36</v>
+      </c>
+      <c r="F277">
+        <v>0</v>
+      </c>
+      <c r="G277">
+        <v>0</v>
+      </c>
+      <c r="H277">
+        <v>1</v>
+      </c>
+      <c r="I277">
+        <v>1</v>
+      </c>
+      <c r="J277">
+        <v>1</v>
+      </c>
+      <c r="K277">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="278" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A278">
+        <v>20240807</v>
+      </c>
+      <c r="B278">
+        <v>47</v>
+      </c>
+      <c r="C278" t="s">
+        <v>2</v>
+      </c>
+      <c r="D278" t="s">
+        <v>12</v>
+      </c>
+      <c r="E278">
+        <v>37</v>
+      </c>
+      <c r="F278">
+        <v>0</v>
+      </c>
+      <c r="G278">
+        <v>0</v>
+      </c>
+      <c r="H278">
+        <v>0</v>
+      </c>
+      <c r="I278">
+        <v>0</v>
+      </c>
+      <c r="J278">
+        <v>0</v>
+      </c>
+      <c r="K278">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A279">
+        <v>20240807</v>
+      </c>
+      <c r="B279">
+        <v>47</v>
+      </c>
+      <c r="C279" t="s">
+        <v>2</v>
+      </c>
+      <c r="D279" t="s">
+        <v>12</v>
+      </c>
+      <c r="E279">
+        <v>38</v>
+      </c>
+      <c r="F279">
+        <v>0</v>
+      </c>
+      <c r="G279">
+        <v>0</v>
+      </c>
+      <c r="H279">
+        <v>1</v>
+      </c>
+      <c r="I279">
+        <v>1</v>
+      </c>
+      <c r="J279">
+        <v>1</v>
+      </c>
+      <c r="K279">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A280">
+        <v>20240807</v>
+      </c>
+      <c r="B280">
+        <v>47</v>
+      </c>
+      <c r="C280" t="s">
+        <v>2</v>
+      </c>
+      <c r="D280" t="s">
+        <v>12</v>
+      </c>
+      <c r="E280">
+        <v>39</v>
+      </c>
+      <c r="F280">
+        <v>0</v>
+      </c>
+      <c r="G280">
+        <v>0</v>
+      </c>
+      <c r="H280">
+        <v>0</v>
+      </c>
+      <c r="I280">
+        <v>0</v>
+      </c>
+      <c r="J280">
+        <v>1</v>
+      </c>
+      <c r="K280">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A281">
+        <v>20240807</v>
+      </c>
+      <c r="B281">
+        <v>47</v>
+      </c>
+      <c r="C281" t="s">
+        <v>2</v>
+      </c>
+      <c r="D281" t="s">
+        <v>12</v>
+      </c>
+      <c r="E281">
+        <v>40</v>
+      </c>
+      <c r="F281">
+        <v>0</v>
+      </c>
+      <c r="G281">
+        <v>0</v>
+      </c>
+      <c r="H281">
+        <v>0</v>
+      </c>
+      <c r="I281">
+        <v>1</v>
+      </c>
+      <c r="J281">
+        <v>1</v>
+      </c>
+      <c r="K281">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A282">
+        <v>20240808</v>
+      </c>
+      <c r="B282">
+        <v>56</v>
+      </c>
+      <c r="C282" t="s">
+        <v>14</v>
+      </c>
+      <c r="D282" t="s">
+        <v>11</v>
+      </c>
+      <c r="E282">
+        <v>1</v>
+      </c>
+      <c r="F282">
+        <v>0</v>
+      </c>
+      <c r="G282">
+        <v>0</v>
+      </c>
+      <c r="H282">
+        <v>0</v>
+      </c>
+      <c r="I282">
+        <v>0</v>
+      </c>
+      <c r="J282">
+        <v>0</v>
+      </c>
+      <c r="K282">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A283">
+        <v>20240808</v>
+      </c>
+      <c r="B283">
+        <v>56</v>
+      </c>
+      <c r="C283" t="s">
+        <v>14</v>
+      </c>
+      <c r="D283" t="s">
+        <v>11</v>
+      </c>
+      <c r="E283">
+        <v>2</v>
+      </c>
+      <c r="F283">
+        <v>0</v>
+      </c>
+      <c r="G283">
+        <v>0</v>
+      </c>
+      <c r="H283">
+        <v>0</v>
+      </c>
+      <c r="I283">
+        <v>0</v>
+      </c>
+      <c r="J283">
+        <v>0</v>
+      </c>
+      <c r="K283">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A284">
+        <v>20240808</v>
+      </c>
+      <c r="B284">
+        <v>56</v>
+      </c>
+      <c r="C284" t="s">
+        <v>14</v>
+      </c>
+      <c r="D284" t="s">
+        <v>11</v>
+      </c>
+      <c r="E284">
+        <v>3</v>
+      </c>
+      <c r="F284">
+        <v>0</v>
+      </c>
+      <c r="G284">
+        <v>0</v>
+      </c>
+      <c r="H284">
+        <v>0</v>
+      </c>
+      <c r="I284">
+        <v>0</v>
+      </c>
+      <c r="J284">
+        <v>0</v>
+      </c>
+      <c r="K284">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A285">
+        <v>20240808</v>
+      </c>
+      <c r="B285">
+        <v>56</v>
+      </c>
+      <c r="C285" t="s">
+        <v>14</v>
+      </c>
+      <c r="D285" t="s">
+        <v>11</v>
+      </c>
+      <c r="E285">
+        <v>4</v>
+      </c>
+      <c r="F285">
+        <v>0</v>
+      </c>
+      <c r="G285">
+        <v>0</v>
+      </c>
+      <c r="H285">
+        <v>0</v>
+      </c>
+      <c r="I285">
+        <v>0</v>
+      </c>
+      <c r="J285">
+        <v>0</v>
+      </c>
+      <c r="K285">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A286">
+        <v>20240808</v>
+      </c>
+      <c r="B286">
+        <v>56</v>
+      </c>
+      <c r="C286" t="s">
+        <v>14</v>
+      </c>
+      <c r="D286" t="s">
+        <v>11</v>
+      </c>
+      <c r="E286">
+        <v>5</v>
+      </c>
+      <c r="F286">
+        <v>0</v>
+      </c>
+      <c r="G286">
+        <v>0</v>
+      </c>
+      <c r="H286">
+        <v>0</v>
+      </c>
+      <c r="I286">
+        <v>0</v>
+      </c>
+      <c r="J286">
+        <v>0</v>
+      </c>
+      <c r="K286">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A287">
+        <v>20240808</v>
+      </c>
+      <c r="B287">
+        <v>56</v>
+      </c>
+      <c r="C287" t="s">
+        <v>14</v>
+      </c>
+      <c r="D287" t="s">
+        <v>11</v>
+      </c>
+      <c r="E287">
+        <v>6</v>
+      </c>
+      <c r="F287">
+        <v>0</v>
+      </c>
+      <c r="G287">
+        <v>0</v>
+      </c>
+      <c r="H287">
+        <v>0</v>
+      </c>
+      <c r="I287">
+        <v>0</v>
+      </c>
+      <c r="J287">
+        <v>0</v>
+      </c>
+      <c r="K287">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A288">
+        <v>20240808</v>
+      </c>
+      <c r="B288">
+        <v>56</v>
+      </c>
+      <c r="C288" t="s">
+        <v>14</v>
+      </c>
+      <c r="D288" t="s">
+        <v>11</v>
+      </c>
+      <c r="E288">
+        <v>7</v>
+      </c>
+      <c r="F288">
+        <v>0</v>
+      </c>
+      <c r="G288">
+        <v>0</v>
+      </c>
+      <c r="H288">
+        <v>0</v>
+      </c>
+      <c r="I288">
+        <v>0</v>
+      </c>
+      <c r="J288">
+        <v>0</v>
+      </c>
+      <c r="K288">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="289" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A289">
+        <v>20240808</v>
+      </c>
+      <c r="B289">
+        <v>56</v>
+      </c>
+      <c r="C289" t="s">
+        <v>14</v>
+      </c>
+      <c r="D289" t="s">
+        <v>11</v>
+      </c>
+      <c r="E289">
+        <v>8</v>
+      </c>
+      <c r="F289">
+        <v>0</v>
+      </c>
+      <c r="G289">
+        <v>0</v>
+      </c>
+      <c r="H289">
+        <v>0</v>
+      </c>
+      <c r="I289">
+        <v>0</v>
+      </c>
+      <c r="J289">
+        <v>0</v>
+      </c>
+      <c r="K289">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A290">
+        <v>20240808</v>
+      </c>
+      <c r="B290">
+        <v>56</v>
+      </c>
+      <c r="C290" t="s">
+        <v>14</v>
+      </c>
+      <c r="D290" t="s">
+        <v>11</v>
+      </c>
+      <c r="E290">
+        <v>9</v>
+      </c>
+      <c r="F290">
+        <v>0</v>
+      </c>
+      <c r="G290">
+        <v>0</v>
+      </c>
+      <c r="H290">
+        <v>0</v>
+      </c>
+      <c r="I290">
+        <v>0</v>
+      </c>
+      <c r="J290">
+        <v>0</v>
+      </c>
+      <c r="K290">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A291">
+        <v>20240808</v>
+      </c>
+      <c r="B291">
+        <v>56</v>
+      </c>
+      <c r="C291" t="s">
+        <v>14</v>
+      </c>
+      <c r="D291" t="s">
+        <v>11</v>
+      </c>
+      <c r="E291">
+        <v>10</v>
+      </c>
+      <c r="F291">
+        <v>0</v>
+      </c>
+      <c r="G291">
+        <v>0</v>
+      </c>
+      <c r="H291">
+        <v>0</v>
+      </c>
+      <c r="I291">
+        <v>0</v>
+      </c>
+      <c r="J291">
+        <v>0</v>
+      </c>
+      <c r="K291">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A292">
+        <v>20240808</v>
+      </c>
+      <c r="B292">
+        <v>56</v>
+      </c>
+      <c r="C292" t="s">
+        <v>14</v>
+      </c>
+      <c r="D292" t="s">
+        <v>11</v>
+      </c>
+      <c r="E292">
+        <v>11</v>
+      </c>
+      <c r="F292">
+        <v>0</v>
+      </c>
+      <c r="G292">
+        <v>0</v>
+      </c>
+      <c r="H292">
+        <v>0</v>
+      </c>
+      <c r="I292">
+        <v>0</v>
+      </c>
+      <c r="J292">
+        <v>0</v>
+      </c>
+      <c r="K292">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A293">
+        <v>20240808</v>
+      </c>
+      <c r="B293">
+        <v>56</v>
+      </c>
+      <c r="C293" t="s">
+        <v>14</v>
+      </c>
+      <c r="D293" t="s">
+        <v>11</v>
+      </c>
+      <c r="E293">
+        <v>12</v>
+      </c>
+      <c r="F293">
+        <v>0</v>
+      </c>
+      <c r="G293">
+        <v>0</v>
+      </c>
+      <c r="H293">
+        <v>0</v>
+      </c>
+      <c r="I293">
+        <v>0</v>
+      </c>
+      <c r="J293">
+        <v>0</v>
+      </c>
+      <c r="K293">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A294">
+        <v>20240808</v>
+      </c>
+      <c r="B294">
+        <v>56</v>
+      </c>
+      <c r="C294" t="s">
+        <v>14</v>
+      </c>
+      <c r="D294" t="s">
+        <v>11</v>
+      </c>
+      <c r="E294">
+        <v>13</v>
+      </c>
+      <c r="F294">
+        <v>0</v>
+      </c>
+      <c r="G294">
+        <v>0</v>
+      </c>
+      <c r="H294">
+        <v>0</v>
+      </c>
+      <c r="I294">
+        <v>0</v>
+      </c>
+      <c r="J294">
+        <v>0</v>
+      </c>
+      <c r="K294">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A295">
+        <v>20240808</v>
+      </c>
+      <c r="B295">
+        <v>56</v>
+      </c>
+      <c r="C295" t="s">
+        <v>14</v>
+      </c>
+      <c r="D295" t="s">
+        <v>11</v>
+      </c>
+      <c r="E295">
+        <v>14</v>
+      </c>
+      <c r="F295">
+        <v>0</v>
+      </c>
+      <c r="G295">
+        <v>0</v>
+      </c>
+      <c r="H295">
+        <v>0</v>
+      </c>
+      <c r="I295">
+        <v>0</v>
+      </c>
+      <c r="J295">
+        <v>0</v>
+      </c>
+      <c r="K295">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A296">
+        <v>20240808</v>
+      </c>
+      <c r="B296">
+        <v>56</v>
+      </c>
+      <c r="C296" t="s">
+        <v>14</v>
+      </c>
+      <c r="D296" t="s">
+        <v>11</v>
+      </c>
+      <c r="E296">
+        <v>15</v>
+      </c>
+      <c r="F296">
+        <v>0</v>
+      </c>
+      <c r="G296">
+        <v>0</v>
+      </c>
+      <c r="H296">
+        <v>0</v>
+      </c>
+      <c r="I296">
+        <v>0</v>
+      </c>
+      <c r="J296">
+        <v>0</v>
+      </c>
+      <c r="K296">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A297">
+        <v>20240808</v>
+      </c>
+      <c r="B297">
+        <v>56</v>
+      </c>
+      <c r="C297" t="s">
+        <v>14</v>
+      </c>
+      <c r="D297" t="s">
+        <v>11</v>
+      </c>
+      <c r="E297">
+        <v>16</v>
+      </c>
+      <c r="F297">
+        <v>0</v>
+      </c>
+      <c r="G297">
+        <v>0</v>
+      </c>
+      <c r="H297">
+        <v>0</v>
+      </c>
+      <c r="I297">
+        <v>0</v>
+      </c>
+      <c r="J297">
+        <v>0</v>
+      </c>
+      <c r="K297">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A298">
+        <v>20240808</v>
+      </c>
+      <c r="B298">
+        <v>56</v>
+      </c>
+      <c r="C298" t="s">
+        <v>14</v>
+      </c>
+      <c r="D298" t="s">
+        <v>11</v>
+      </c>
+      <c r="E298">
+        <v>17</v>
+      </c>
+      <c r="F298">
+        <v>0</v>
+      </c>
+      <c r="G298">
+        <v>0</v>
+      </c>
+      <c r="H298">
+        <v>0</v>
+      </c>
+      <c r="I298">
+        <v>0</v>
+      </c>
+      <c r="J298">
+        <v>0</v>
+      </c>
+      <c r="K298">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="299" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A299">
+        <v>20240808</v>
+      </c>
+      <c r="B299">
+        <v>56</v>
+      </c>
+      <c r="C299" t="s">
+        <v>14</v>
+      </c>
+      <c r="D299" t="s">
+        <v>11</v>
+      </c>
+      <c r="E299">
+        <v>18</v>
+      </c>
+      <c r="F299">
+        <v>0</v>
+      </c>
+      <c r="G299">
+        <v>0</v>
+      </c>
+      <c r="H299">
+        <v>0</v>
+      </c>
+      <c r="I299">
+        <v>0</v>
+      </c>
+      <c r="J299">
+        <v>0</v>
+      </c>
+      <c r="K299">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="300" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A300">
+        <v>20240808</v>
+      </c>
+      <c r="B300">
+        <v>56</v>
+      </c>
+      <c r="C300" t="s">
+        <v>14</v>
+      </c>
+      <c r="D300" t="s">
+        <v>11</v>
+      </c>
+      <c r="E300">
+        <v>19</v>
+      </c>
+      <c r="F300">
+        <v>0</v>
+      </c>
+      <c r="G300">
+        <v>0</v>
+      </c>
+      <c r="H300">
+        <v>0</v>
+      </c>
+      <c r="I300">
+        <v>0</v>
+      </c>
+      <c r="J300">
+        <v>0</v>
+      </c>
+      <c r="K300">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A301">
+        <v>20240808</v>
+      </c>
+      <c r="B301">
+        <v>56</v>
+      </c>
+      <c r="C301" t="s">
+        <v>14</v>
+      </c>
+      <c r="D301" t="s">
+        <v>11</v>
+      </c>
+      <c r="E301">
+        <v>20</v>
+      </c>
+      <c r="F301">
+        <v>0</v>
+      </c>
+      <c r="G301">
+        <v>0</v>
+      </c>
+      <c r="H301">
+        <v>0</v>
+      </c>
+      <c r="I301">
+        <v>0</v>
+      </c>
+      <c r="J301">
+        <v>0</v>
+      </c>
+      <c r="K301">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A302">
+        <v>20240808</v>
+      </c>
+      <c r="B302">
+        <v>56</v>
+      </c>
+      <c r="C302" t="s">
+        <v>14</v>
+      </c>
+      <c r="D302" t="s">
+        <v>12</v>
+      </c>
+      <c r="E302">
+        <v>21</v>
+      </c>
+      <c r="F302">
+        <v>0</v>
+      </c>
+      <c r="G302">
+        <v>0</v>
+      </c>
+      <c r="H302">
+        <v>0</v>
+      </c>
+      <c r="I302">
+        <v>0</v>
+      </c>
+      <c r="J302">
+        <v>0</v>
+      </c>
+      <c r="K302">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="303" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A303">
+        <v>20240808</v>
+      </c>
+      <c r="B303">
+        <v>56</v>
+      </c>
+      <c r="C303" t="s">
+        <v>14</v>
+      </c>
+      <c r="D303" t="s">
+        <v>12</v>
+      </c>
+      <c r="E303">
+        <v>22</v>
+      </c>
+      <c r="F303">
+        <v>0</v>
+      </c>
+      <c r="G303">
+        <v>0</v>
+      </c>
+      <c r="H303">
+        <v>1</v>
+      </c>
+      <c r="I303">
+        <v>1</v>
+      </c>
+      <c r="J303">
+        <v>1</v>
+      </c>
+      <c r="K303">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="304" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A304">
+        <v>20240808</v>
+      </c>
+      <c r="B304">
+        <v>56</v>
+      </c>
+      <c r="C304" t="s">
+        <v>14</v>
+      </c>
+      <c r="D304" t="s">
+        <v>12</v>
+      </c>
+      <c r="E304">
+        <v>23</v>
+      </c>
+      <c r="F304">
+        <v>0</v>
+      </c>
+      <c r="G304">
+        <v>0</v>
+      </c>
+      <c r="H304">
+        <v>0</v>
+      </c>
+      <c r="I304">
+        <v>0</v>
+      </c>
+      <c r="J304">
+        <v>0</v>
+      </c>
+      <c r="K304">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="305" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A305">
+        <v>20240808</v>
+      </c>
+      <c r="B305">
+        <v>56</v>
+      </c>
+      <c r="C305" t="s">
+        <v>14</v>
+      </c>
+      <c r="D305" t="s">
+        <v>12</v>
+      </c>
+      <c r="E305">
+        <v>24</v>
+      </c>
+      <c r="F305">
+        <v>0</v>
+      </c>
+      <c r="G305">
+        <v>0</v>
+      </c>
+      <c r="H305">
+        <v>0</v>
+      </c>
+      <c r="I305">
+        <v>0</v>
+      </c>
+      <c r="J305">
+        <v>0</v>
+      </c>
+      <c r="K305">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A306">
+        <v>20240808</v>
+      </c>
+      <c r="B306">
+        <v>56</v>
+      </c>
+      <c r="C306" t="s">
+        <v>14</v>
+      </c>
+      <c r="D306" t="s">
+        <v>12</v>
+      </c>
+      <c r="E306">
+        <v>25</v>
+      </c>
+      <c r="F306">
+        <v>0</v>
+      </c>
+      <c r="G306">
+        <v>0</v>
+      </c>
+      <c r="H306">
+        <v>0</v>
+      </c>
+      <c r="I306">
+        <v>0</v>
+      </c>
+      <c r="J306">
+        <v>0</v>
+      </c>
+      <c r="K306">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="307" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A307">
+        <v>20240808</v>
+      </c>
+      <c r="B307">
+        <v>56</v>
+      </c>
+      <c r="C307" t="s">
+        <v>14</v>
+      </c>
+      <c r="D307" t="s">
+        <v>12</v>
+      </c>
+      <c r="E307">
+        <v>26</v>
+      </c>
+      <c r="F307">
+        <v>0</v>
+      </c>
+      <c r="G307">
+        <v>0</v>
+      </c>
+      <c r="H307">
+        <v>0</v>
+      </c>
+      <c r="I307">
+        <v>0</v>
+      </c>
+      <c r="J307">
+        <v>0</v>
+      </c>
+      <c r="K307">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="308" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A308">
+        <v>20240808</v>
+      </c>
+      <c r="B308">
+        <v>56</v>
+      </c>
+      <c r="C308" t="s">
+        <v>14</v>
+      </c>
+      <c r="D308" t="s">
+        <v>12</v>
+      </c>
+      <c r="E308">
+        <v>27</v>
+      </c>
+      <c r="F308">
+        <v>0</v>
+      </c>
+      <c r="G308">
+        <v>0</v>
+      </c>
+      <c r="H308">
+        <v>0</v>
+      </c>
+      <c r="I308">
+        <v>0</v>
+      </c>
+      <c r="J308">
+        <v>0</v>
+      </c>
+      <c r="K308">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A309">
+        <v>20240808</v>
+      </c>
+      <c r="B309">
+        <v>56</v>
+      </c>
+      <c r="C309" t="s">
+        <v>14</v>
+      </c>
+      <c r="D309" t="s">
+        <v>12</v>
+      </c>
+      <c r="E309">
+        <v>28</v>
+      </c>
+      <c r="F309">
+        <v>0</v>
+      </c>
+      <c r="G309">
+        <v>0</v>
+      </c>
+      <c r="H309">
+        <v>1</v>
+      </c>
+      <c r="I309">
+        <v>1</v>
+      </c>
+      <c r="J309">
+        <v>1</v>
+      </c>
+      <c r="K309">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="310" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A310">
+        <v>20240808</v>
+      </c>
+      <c r="B310">
+        <v>56</v>
+      </c>
+      <c r="C310" t="s">
+        <v>14</v>
+      </c>
+      <c r="D310" t="s">
+        <v>12</v>
+      </c>
+      <c r="E310">
+        <v>29</v>
+      </c>
+      <c r="F310">
+        <v>0</v>
+      </c>
+      <c r="G310">
+        <v>0</v>
+      </c>
+      <c r="H310">
+        <v>0</v>
+      </c>
+      <c r="I310">
+        <v>0</v>
+      </c>
+      <c r="J310">
+        <v>0</v>
+      </c>
+      <c r="K310">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="311" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A311">
+        <v>20240808</v>
+      </c>
+      <c r="B311">
+        <v>56</v>
+      </c>
+      <c r="C311" t="s">
+        <v>14</v>
+      </c>
+      <c r="D311" t="s">
+        <v>12</v>
+      </c>
+      <c r="E311">
+        <v>30</v>
+      </c>
+      <c r="F311">
+        <v>0</v>
+      </c>
+      <c r="G311">
+        <v>0</v>
+      </c>
+      <c r="H311">
+        <v>0</v>
+      </c>
+      <c r="I311">
+        <v>0</v>
+      </c>
+      <c r="J311">
+        <v>0</v>
+      </c>
+      <c r="K311">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A312">
+        <v>20240808</v>
+      </c>
+      <c r="B312">
+        <v>56</v>
+      </c>
+      <c r="C312" t="s">
+        <v>14</v>
+      </c>
+      <c r="D312" t="s">
+        <v>12</v>
+      </c>
+      <c r="E312">
+        <v>31</v>
+      </c>
+      <c r="F312">
+        <v>0</v>
+      </c>
+      <c r="G312">
+        <v>0</v>
+      </c>
+      <c r="H312">
+        <v>0</v>
+      </c>
+      <c r="I312">
+        <v>0</v>
+      </c>
+      <c r="J312">
+        <v>0</v>
+      </c>
+      <c r="K312">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A313">
+        <v>20240808</v>
+      </c>
+      <c r="B313">
+        <v>56</v>
+      </c>
+      <c r="C313" t="s">
+        <v>14</v>
+      </c>
+      <c r="D313" t="s">
+        <v>12</v>
+      </c>
+      <c r="E313">
+        <v>32</v>
+      </c>
+      <c r="F313">
+        <v>0</v>
+      </c>
+      <c r="G313">
+        <v>0</v>
+      </c>
+      <c r="H313">
+        <v>0</v>
+      </c>
+      <c r="I313">
+        <v>0</v>
+      </c>
+      <c r="J313">
+        <v>0</v>
+      </c>
+      <c r="K313">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="314" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A314">
+        <v>20240808</v>
+      </c>
+      <c r="B314">
+        <v>56</v>
+      </c>
+      <c r="C314" t="s">
+        <v>14</v>
+      </c>
+      <c r="D314" t="s">
+        <v>12</v>
+      </c>
+      <c r="E314">
+        <v>33</v>
+      </c>
+      <c r="F314">
+        <v>0</v>
+      </c>
+      <c r="G314">
+        <v>1</v>
+      </c>
+      <c r="H314">
+        <v>1</v>
+      </c>
+      <c r="I314">
+        <v>1</v>
+      </c>
+      <c r="J314">
+        <v>1</v>
+      </c>
+      <c r="K314">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="315" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A315">
+        <v>20240808</v>
+      </c>
+      <c r="B315">
+        <v>56</v>
+      </c>
+      <c r="C315" t="s">
+        <v>14</v>
+      </c>
+      <c r="D315" t="s">
+        <v>12</v>
+      </c>
+      <c r="E315">
+        <v>34</v>
+      </c>
+      <c r="F315">
+        <v>0</v>
+      </c>
+      <c r="G315">
+        <v>0</v>
+      </c>
+      <c r="H315">
+        <v>1</v>
+      </c>
+      <c r="I315">
+        <v>1</v>
+      </c>
+      <c r="J315">
+        <v>1</v>
+      </c>
+      <c r="K315">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A316">
+        <v>20240808</v>
+      </c>
+      <c r="B316">
+        <v>56</v>
+      </c>
+      <c r="C316" t="s">
+        <v>14</v>
+      </c>
+      <c r="D316" t="s">
+        <v>12</v>
+      </c>
+      <c r="E316">
+        <v>35</v>
+      </c>
+      <c r="F316">
+        <v>0</v>
+      </c>
+      <c r="G316">
+        <v>0</v>
+      </c>
+      <c r="H316">
+        <v>0</v>
+      </c>
+      <c r="I316">
+        <v>0</v>
+      </c>
+      <c r="J316">
+        <v>1</v>
+      </c>
+      <c r="K316">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="317" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A317">
+        <v>20240808</v>
+      </c>
+      <c r="B317">
+        <v>56</v>
+      </c>
+      <c r="C317" t="s">
+        <v>14</v>
+      </c>
+      <c r="D317" t="s">
+        <v>12</v>
+      </c>
+      <c r="E317">
+        <v>36</v>
+      </c>
+      <c r="F317">
+        <v>0</v>
+      </c>
+      <c r="G317">
+        <v>0</v>
+      </c>
+      <c r="H317">
+        <v>1</v>
+      </c>
+      <c r="I317">
+        <v>1</v>
+      </c>
+      <c r="J317">
+        <v>1</v>
+      </c>
+      <c r="K317">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="318" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A318">
+        <v>20240808</v>
+      </c>
+      <c r="B318">
+        <v>56</v>
+      </c>
+      <c r="C318" t="s">
+        <v>14</v>
+      </c>
+      <c r="D318" t="s">
+        <v>12</v>
+      </c>
+      <c r="E318">
+        <v>37</v>
+      </c>
+      <c r="F318">
+        <v>0</v>
+      </c>
+      <c r="G318">
+        <v>0</v>
+      </c>
+      <c r="H318">
+        <v>0</v>
+      </c>
+      <c r="I318">
+        <v>1</v>
+      </c>
+      <c r="J318">
+        <v>1</v>
+      </c>
+      <c r="K318">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="319" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A319">
+        <v>20240808</v>
+      </c>
+      <c r="B319">
+        <v>56</v>
+      </c>
+      <c r="C319" t="s">
+        <v>14</v>
+      </c>
+      <c r="D319" t="s">
+        <v>12</v>
+      </c>
+      <c r="E319">
+        <v>38</v>
+      </c>
+      <c r="F319">
+        <v>0</v>
+      </c>
+      <c r="G319">
+        <v>0</v>
+      </c>
+      <c r="H319">
+        <v>1</v>
+      </c>
+      <c r="I319">
+        <v>1</v>
+      </c>
+      <c r="J319">
+        <v>1</v>
+      </c>
+      <c r="K319">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="320" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A320">
+        <v>20240808</v>
+      </c>
+      <c r="B320">
+        <v>56</v>
+      </c>
+      <c r="C320" t="s">
+        <v>14</v>
+      </c>
+      <c r="D320" t="s">
+        <v>12</v>
+      </c>
+      <c r="E320">
+        <v>39</v>
+      </c>
+      <c r="F320">
+        <v>0</v>
+      </c>
+      <c r="G320">
+        <v>0</v>
+      </c>
+      <c r="H320">
+        <v>0</v>
+      </c>
+      <c r="I320">
+        <v>0</v>
+      </c>
+      <c r="J320">
+        <v>1</v>
+      </c>
+      <c r="K320">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="321" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A321">
+        <v>20240808</v>
+      </c>
+      <c r="B321">
+        <v>56</v>
+      </c>
+      <c r="C321" t="s">
+        <v>14</v>
+      </c>
+      <c r="D321" t="s">
+        <v>12</v>
+      </c>
+      <c r="E321">
+        <v>40</v>
+      </c>
+      <c r="F321">
+        <v>0</v>
+      </c>
+      <c r="G321">
+        <v>0</v>
+      </c>
+      <c r="H321">
+        <v>0</v>
+      </c>
+      <c r="I321">
+        <v>0</v>
+      </c>
+      <c r="J321">
+        <v>0</v>
+      </c>
+      <c r="K321">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated resazurin survival as of 8/14
</commit_message>
<xml_diff>
--- a/data/survival/survival_resazurin.xlsx
+++ b/data/survival/survival_resazurin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/10K-seed-Cgigas/data/survival/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6C1C3D-CF74-A744-8733-A060CF53787D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474F4954-B4C6-4F41-910B-C164FD376379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="760" windowWidth="18160" windowHeight="17720" xr2:uid="{FF76C7E6-3408-934E-9F62-D1FDE39EF6F8}"/>
+    <workbookView xWindow="-620" yWindow="760" windowWidth="18160" windowHeight="17720" xr2:uid="{FF76C7E6-3408-934E-9F62-D1FDE39EF6F8}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="17">
   <si>
     <t>date.resazurin</t>
   </si>
@@ -459,11 +459,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE0A6E7-C44F-C349-A3CE-3BF585EE18ED}">
-  <dimension ref="A1:K361"/>
+  <dimension ref="A1:K401"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A329" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K355" sqref="K355"/>
+      <pane ySplit="1" topLeftCell="A367" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K401" sqref="K401"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13105,6 +13105,1406 @@
         <v>1</v>
       </c>
       <c r="K361">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="362" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A362">
+        <v>20240813</v>
+      </c>
+      <c r="B362">
+        <v>49</v>
+      </c>
+      <c r="C362" t="s">
+        <v>16</v>
+      </c>
+      <c r="D362" t="s">
+        <v>11</v>
+      </c>
+      <c r="E362">
+        <v>1</v>
+      </c>
+      <c r="F362">
+        <v>0</v>
+      </c>
+      <c r="G362">
+        <v>0</v>
+      </c>
+      <c r="H362">
+        <v>0</v>
+      </c>
+      <c r="I362">
+        <v>0</v>
+      </c>
+      <c r="J362">
+        <v>0</v>
+      </c>
+      <c r="K362">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="363" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A363">
+        <v>20240813</v>
+      </c>
+      <c r="B363">
+        <v>49</v>
+      </c>
+      <c r="C363" t="s">
+        <v>16</v>
+      </c>
+      <c r="D363" t="s">
+        <v>11</v>
+      </c>
+      <c r="E363">
+        <v>2</v>
+      </c>
+      <c r="F363">
+        <v>0</v>
+      </c>
+      <c r="G363">
+        <v>0</v>
+      </c>
+      <c r="H363">
+        <v>0</v>
+      </c>
+      <c r="I363">
+        <v>0</v>
+      </c>
+      <c r="J363">
+        <v>0</v>
+      </c>
+      <c r="K363">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="364" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A364">
+        <v>20240813</v>
+      </c>
+      <c r="B364">
+        <v>49</v>
+      </c>
+      <c r="C364" t="s">
+        <v>16</v>
+      </c>
+      <c r="D364" t="s">
+        <v>11</v>
+      </c>
+      <c r="E364">
+        <v>3</v>
+      </c>
+      <c r="F364">
+        <v>0</v>
+      </c>
+      <c r="G364">
+        <v>0</v>
+      </c>
+      <c r="H364">
+        <v>0</v>
+      </c>
+      <c r="I364">
+        <v>0</v>
+      </c>
+      <c r="J364">
+        <v>0</v>
+      </c>
+      <c r="K364">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="365" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A365">
+        <v>20240813</v>
+      </c>
+      <c r="B365">
+        <v>49</v>
+      </c>
+      <c r="C365" t="s">
+        <v>16</v>
+      </c>
+      <c r="D365" t="s">
+        <v>11</v>
+      </c>
+      <c r="E365">
+        <v>4</v>
+      </c>
+      <c r="F365">
+        <v>0</v>
+      </c>
+      <c r="G365">
+        <v>0</v>
+      </c>
+      <c r="H365">
+        <v>0</v>
+      </c>
+      <c r="I365">
+        <v>0</v>
+      </c>
+      <c r="J365">
+        <v>0</v>
+      </c>
+      <c r="K365">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="366" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A366">
+        <v>20240813</v>
+      </c>
+      <c r="B366">
+        <v>49</v>
+      </c>
+      <c r="C366" t="s">
+        <v>16</v>
+      </c>
+      <c r="D366" t="s">
+        <v>11</v>
+      </c>
+      <c r="E366">
+        <v>5</v>
+      </c>
+      <c r="F366">
+        <v>0</v>
+      </c>
+      <c r="G366">
+        <v>0</v>
+      </c>
+      <c r="H366">
+        <v>0</v>
+      </c>
+      <c r="I366">
+        <v>0</v>
+      </c>
+      <c r="J366">
+        <v>0</v>
+      </c>
+      <c r="K366">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="367" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A367">
+        <v>20240813</v>
+      </c>
+      <c r="B367">
+        <v>49</v>
+      </c>
+      <c r="C367" t="s">
+        <v>16</v>
+      </c>
+      <c r="D367" t="s">
+        <v>11</v>
+      </c>
+      <c r="E367">
+        <v>6</v>
+      </c>
+      <c r="F367">
+        <v>0</v>
+      </c>
+      <c r="G367">
+        <v>0</v>
+      </c>
+      <c r="H367">
+        <v>0</v>
+      </c>
+      <c r="I367">
+        <v>0</v>
+      </c>
+      <c r="J367">
+        <v>0</v>
+      </c>
+      <c r="K367">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="368" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A368">
+        <v>20240813</v>
+      </c>
+      <c r="B368">
+        <v>49</v>
+      </c>
+      <c r="C368" t="s">
+        <v>16</v>
+      </c>
+      <c r="D368" t="s">
+        <v>11</v>
+      </c>
+      <c r="E368">
+        <v>7</v>
+      </c>
+      <c r="F368">
+        <v>0</v>
+      </c>
+      <c r="G368">
+        <v>0</v>
+      </c>
+      <c r="H368">
+        <v>0</v>
+      </c>
+      <c r="I368">
+        <v>0</v>
+      </c>
+      <c r="J368">
+        <v>0</v>
+      </c>
+      <c r="K368">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="369" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A369">
+        <v>20240813</v>
+      </c>
+      <c r="B369">
+        <v>49</v>
+      </c>
+      <c r="C369" t="s">
+        <v>16</v>
+      </c>
+      <c r="D369" t="s">
+        <v>11</v>
+      </c>
+      <c r="E369">
+        <v>8</v>
+      </c>
+      <c r="F369">
+        <v>0</v>
+      </c>
+      <c r="G369">
+        <v>0</v>
+      </c>
+      <c r="H369">
+        <v>0</v>
+      </c>
+      <c r="I369">
+        <v>0</v>
+      </c>
+      <c r="J369">
+        <v>1</v>
+      </c>
+      <c r="K369">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="370" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A370">
+        <v>20240813</v>
+      </c>
+      <c r="B370">
+        <v>49</v>
+      </c>
+      <c r="C370" t="s">
+        <v>16</v>
+      </c>
+      <c r="D370" t="s">
+        <v>11</v>
+      </c>
+      <c r="E370">
+        <v>9</v>
+      </c>
+      <c r="F370">
+        <v>0</v>
+      </c>
+      <c r="G370">
+        <v>0</v>
+      </c>
+      <c r="H370">
+        <v>0</v>
+      </c>
+      <c r="I370">
+        <v>0</v>
+      </c>
+      <c r="J370">
+        <v>0</v>
+      </c>
+      <c r="K370">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="371" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A371">
+        <v>20240813</v>
+      </c>
+      <c r="B371">
+        <v>49</v>
+      </c>
+      <c r="C371" t="s">
+        <v>16</v>
+      </c>
+      <c r="D371" t="s">
+        <v>11</v>
+      </c>
+      <c r="E371">
+        <v>10</v>
+      </c>
+      <c r="F371">
+        <v>0</v>
+      </c>
+      <c r="G371">
+        <v>0</v>
+      </c>
+      <c r="H371">
+        <v>0</v>
+      </c>
+      <c r="I371">
+        <v>0</v>
+      </c>
+      <c r="J371">
+        <v>0</v>
+      </c>
+      <c r="K371">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="372" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A372">
+        <v>20240813</v>
+      </c>
+      <c r="B372">
+        <v>49</v>
+      </c>
+      <c r="C372" t="s">
+        <v>16</v>
+      </c>
+      <c r="D372" t="s">
+        <v>11</v>
+      </c>
+      <c r="E372">
+        <v>11</v>
+      </c>
+      <c r="F372">
+        <v>0</v>
+      </c>
+      <c r="G372">
+        <v>0</v>
+      </c>
+      <c r="H372">
+        <v>0</v>
+      </c>
+      <c r="I372">
+        <v>0</v>
+      </c>
+      <c r="J372">
+        <v>0</v>
+      </c>
+      <c r="K372">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="373" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A373">
+        <v>20240813</v>
+      </c>
+      <c r="B373">
+        <v>49</v>
+      </c>
+      <c r="C373" t="s">
+        <v>16</v>
+      </c>
+      <c r="D373" t="s">
+        <v>11</v>
+      </c>
+      <c r="E373">
+        <v>12</v>
+      </c>
+      <c r="F373">
+        <v>0</v>
+      </c>
+      <c r="G373">
+        <v>0</v>
+      </c>
+      <c r="H373">
+        <v>0</v>
+      </c>
+      <c r="I373">
+        <v>0</v>
+      </c>
+      <c r="J373">
+        <v>0</v>
+      </c>
+      <c r="K373">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="374" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A374">
+        <v>20240813</v>
+      </c>
+      <c r="B374">
+        <v>49</v>
+      </c>
+      <c r="C374" t="s">
+        <v>16</v>
+      </c>
+      <c r="D374" t="s">
+        <v>11</v>
+      </c>
+      <c r="E374">
+        <v>13</v>
+      </c>
+      <c r="F374">
+        <v>0</v>
+      </c>
+      <c r="G374">
+        <v>0</v>
+      </c>
+      <c r="H374">
+        <v>0</v>
+      </c>
+      <c r="I374">
+        <v>0</v>
+      </c>
+      <c r="J374">
+        <v>0</v>
+      </c>
+      <c r="K374">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="375" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A375">
+        <v>20240813</v>
+      </c>
+      <c r="B375">
+        <v>49</v>
+      </c>
+      <c r="C375" t="s">
+        <v>16</v>
+      </c>
+      <c r="D375" t="s">
+        <v>11</v>
+      </c>
+      <c r="E375">
+        <v>14</v>
+      </c>
+      <c r="F375">
+        <v>0</v>
+      </c>
+      <c r="G375">
+        <v>0</v>
+      </c>
+      <c r="H375">
+        <v>0</v>
+      </c>
+      <c r="I375">
+        <v>0</v>
+      </c>
+      <c r="J375">
+        <v>0</v>
+      </c>
+      <c r="K375">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="376" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A376">
+        <v>20240813</v>
+      </c>
+      <c r="B376">
+        <v>49</v>
+      </c>
+      <c r="C376" t="s">
+        <v>16</v>
+      </c>
+      <c r="D376" t="s">
+        <v>11</v>
+      </c>
+      <c r="E376">
+        <v>15</v>
+      </c>
+      <c r="F376">
+        <v>0</v>
+      </c>
+      <c r="G376">
+        <v>0</v>
+      </c>
+      <c r="H376">
+        <v>0</v>
+      </c>
+      <c r="I376">
+        <v>0</v>
+      </c>
+      <c r="J376">
+        <v>0</v>
+      </c>
+      <c r="K376">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="377" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A377">
+        <v>20240813</v>
+      </c>
+      <c r="B377">
+        <v>49</v>
+      </c>
+      <c r="C377" t="s">
+        <v>16</v>
+      </c>
+      <c r="D377" t="s">
+        <v>11</v>
+      </c>
+      <c r="E377">
+        <v>16</v>
+      </c>
+      <c r="F377">
+        <v>0</v>
+      </c>
+      <c r="G377">
+        <v>0</v>
+      </c>
+      <c r="H377">
+        <v>0</v>
+      </c>
+      <c r="I377">
+        <v>0</v>
+      </c>
+      <c r="J377">
+        <v>0</v>
+      </c>
+      <c r="K377">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="378" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A378">
+        <v>20240813</v>
+      </c>
+      <c r="B378">
+        <v>49</v>
+      </c>
+      <c r="C378" t="s">
+        <v>16</v>
+      </c>
+      <c r="D378" t="s">
+        <v>11</v>
+      </c>
+      <c r="E378">
+        <v>17</v>
+      </c>
+      <c r="F378">
+        <v>0</v>
+      </c>
+      <c r="G378">
+        <v>0</v>
+      </c>
+      <c r="H378">
+        <v>0</v>
+      </c>
+      <c r="I378">
+        <v>0</v>
+      </c>
+      <c r="J378">
+        <v>0</v>
+      </c>
+      <c r="K378">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="379" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A379">
+        <v>20240813</v>
+      </c>
+      <c r="B379">
+        <v>49</v>
+      </c>
+      <c r="C379" t="s">
+        <v>16</v>
+      </c>
+      <c r="D379" t="s">
+        <v>11</v>
+      </c>
+      <c r="E379">
+        <v>18</v>
+      </c>
+      <c r="F379">
+        <v>0</v>
+      </c>
+      <c r="G379">
+        <v>0</v>
+      </c>
+      <c r="H379">
+        <v>0</v>
+      </c>
+      <c r="I379">
+        <v>0</v>
+      </c>
+      <c r="J379">
+        <v>0</v>
+      </c>
+      <c r="K379">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="380" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A380">
+        <v>20240813</v>
+      </c>
+      <c r="B380">
+        <v>49</v>
+      </c>
+      <c r="C380" t="s">
+        <v>16</v>
+      </c>
+      <c r="D380" t="s">
+        <v>11</v>
+      </c>
+      <c r="E380">
+        <v>19</v>
+      </c>
+      <c r="F380">
+        <v>0</v>
+      </c>
+      <c r="G380">
+        <v>0</v>
+      </c>
+      <c r="H380">
+        <v>0</v>
+      </c>
+      <c r="I380">
+        <v>0</v>
+      </c>
+      <c r="J380">
+        <v>0</v>
+      </c>
+      <c r="K380">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="381" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A381">
+        <v>20240813</v>
+      </c>
+      <c r="B381">
+        <v>49</v>
+      </c>
+      <c r="C381" t="s">
+        <v>16</v>
+      </c>
+      <c r="D381" t="s">
+        <v>11</v>
+      </c>
+      <c r="E381">
+        <v>20</v>
+      </c>
+      <c r="F381">
+        <v>0</v>
+      </c>
+      <c r="G381">
+        <v>0</v>
+      </c>
+      <c r="H381">
+        <v>0</v>
+      </c>
+      <c r="I381">
+        <v>0</v>
+      </c>
+      <c r="J381">
+        <v>0</v>
+      </c>
+      <c r="K381">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="382" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A382">
+        <v>20240813</v>
+      </c>
+      <c r="B382">
+        <v>49</v>
+      </c>
+      <c r="C382" t="s">
+        <v>16</v>
+      </c>
+      <c r="D382" t="s">
+        <v>12</v>
+      </c>
+      <c r="E382">
+        <v>21</v>
+      </c>
+      <c r="F382">
+        <v>0</v>
+      </c>
+      <c r="G382">
+        <v>0</v>
+      </c>
+      <c r="H382">
+        <v>0</v>
+      </c>
+      <c r="I382">
+        <v>0</v>
+      </c>
+      <c r="J382">
+        <v>0</v>
+      </c>
+      <c r="K382">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="383" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A383">
+        <v>20240813</v>
+      </c>
+      <c r="B383">
+        <v>49</v>
+      </c>
+      <c r="C383" t="s">
+        <v>16</v>
+      </c>
+      <c r="D383" t="s">
+        <v>12</v>
+      </c>
+      <c r="E383">
+        <v>22</v>
+      </c>
+      <c r="F383">
+        <v>0</v>
+      </c>
+      <c r="G383">
+        <v>0</v>
+      </c>
+      <c r="H383">
+        <v>1</v>
+      </c>
+      <c r="I383">
+        <v>1</v>
+      </c>
+      <c r="J383">
+        <v>1</v>
+      </c>
+      <c r="K383">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="384" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A384">
+        <v>20240813</v>
+      </c>
+      <c r="B384">
+        <v>49</v>
+      </c>
+      <c r="C384" t="s">
+        <v>16</v>
+      </c>
+      <c r="D384" t="s">
+        <v>12</v>
+      </c>
+      <c r="E384">
+        <v>23</v>
+      </c>
+      <c r="F384">
+        <v>0</v>
+      </c>
+      <c r="G384">
+        <v>0</v>
+      </c>
+      <c r="H384">
+        <v>0</v>
+      </c>
+      <c r="I384">
+        <v>0</v>
+      </c>
+      <c r="J384">
+        <v>0</v>
+      </c>
+      <c r="K384">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="385" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A385">
+        <v>20240813</v>
+      </c>
+      <c r="B385">
+        <v>49</v>
+      </c>
+      <c r="C385" t="s">
+        <v>16</v>
+      </c>
+      <c r="D385" t="s">
+        <v>12</v>
+      </c>
+      <c r="E385">
+        <v>24</v>
+      </c>
+      <c r="F385">
+        <v>0</v>
+      </c>
+      <c r="G385">
+        <v>0</v>
+      </c>
+      <c r="H385">
+        <v>0</v>
+      </c>
+      <c r="I385">
+        <v>0</v>
+      </c>
+      <c r="J385">
+        <v>0</v>
+      </c>
+      <c r="K385">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="386" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A386">
+        <v>20240813</v>
+      </c>
+      <c r="B386">
+        <v>49</v>
+      </c>
+      <c r="C386" t="s">
+        <v>16</v>
+      </c>
+      <c r="D386" t="s">
+        <v>12</v>
+      </c>
+      <c r="E386">
+        <v>25</v>
+      </c>
+      <c r="F386">
+        <v>0</v>
+      </c>
+      <c r="G386">
+        <v>0</v>
+      </c>
+      <c r="H386">
+        <v>1</v>
+      </c>
+      <c r="I386">
+        <v>1</v>
+      </c>
+      <c r="J386">
+        <v>1</v>
+      </c>
+      <c r="K386">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="387" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A387">
+        <v>20240813</v>
+      </c>
+      <c r="B387">
+        <v>49</v>
+      </c>
+      <c r="C387" t="s">
+        <v>16</v>
+      </c>
+      <c r="D387" t="s">
+        <v>12</v>
+      </c>
+      <c r="E387">
+        <v>26</v>
+      </c>
+      <c r="F387">
+        <v>0</v>
+      </c>
+      <c r="G387">
+        <v>0</v>
+      </c>
+      <c r="H387">
+        <v>0</v>
+      </c>
+      <c r="I387">
+        <v>0</v>
+      </c>
+      <c r="J387">
+        <v>0</v>
+      </c>
+      <c r="K387">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="388" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A388">
+        <v>20240813</v>
+      </c>
+      <c r="B388">
+        <v>49</v>
+      </c>
+      <c r="C388" t="s">
+        <v>16</v>
+      </c>
+      <c r="D388" t="s">
+        <v>12</v>
+      </c>
+      <c r="E388">
+        <v>27</v>
+      </c>
+      <c r="F388">
+        <v>0</v>
+      </c>
+      <c r="G388">
+        <v>0</v>
+      </c>
+      <c r="H388">
+        <v>1</v>
+      </c>
+      <c r="I388">
+        <v>1</v>
+      </c>
+      <c r="J388">
+        <v>1</v>
+      </c>
+      <c r="K388">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="389" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A389">
+        <v>20240813</v>
+      </c>
+      <c r="B389">
+        <v>49</v>
+      </c>
+      <c r="C389" t="s">
+        <v>16</v>
+      </c>
+      <c r="D389" t="s">
+        <v>12</v>
+      </c>
+      <c r="E389">
+        <v>28</v>
+      </c>
+      <c r="F389">
+        <v>0</v>
+      </c>
+      <c r="G389">
+        <v>0</v>
+      </c>
+      <c r="H389">
+        <v>1</v>
+      </c>
+      <c r="I389">
+        <v>1</v>
+      </c>
+      <c r="J389">
+        <v>1</v>
+      </c>
+      <c r="K389">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="390" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A390">
+        <v>20240813</v>
+      </c>
+      <c r="B390">
+        <v>49</v>
+      </c>
+      <c r="C390" t="s">
+        <v>16</v>
+      </c>
+      <c r="D390" t="s">
+        <v>12</v>
+      </c>
+      <c r="E390">
+        <v>29</v>
+      </c>
+      <c r="F390">
+        <v>0</v>
+      </c>
+      <c r="G390">
+        <v>0</v>
+      </c>
+      <c r="H390">
+        <v>1</v>
+      </c>
+      <c r="I390">
+        <v>1</v>
+      </c>
+      <c r="J390">
+        <v>1</v>
+      </c>
+      <c r="K390">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="391" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A391">
+        <v>20240813</v>
+      </c>
+      <c r="B391">
+        <v>49</v>
+      </c>
+      <c r="C391" t="s">
+        <v>16</v>
+      </c>
+      <c r="D391" t="s">
+        <v>12</v>
+      </c>
+      <c r="E391">
+        <v>30</v>
+      </c>
+      <c r="F391">
+        <v>0</v>
+      </c>
+      <c r="G391">
+        <v>0</v>
+      </c>
+      <c r="H391">
+        <v>1</v>
+      </c>
+      <c r="I391">
+        <v>1</v>
+      </c>
+      <c r="J391">
+        <v>1</v>
+      </c>
+      <c r="K391">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="392" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A392">
+        <v>20240813</v>
+      </c>
+      <c r="B392">
+        <v>49</v>
+      </c>
+      <c r="C392" t="s">
+        <v>16</v>
+      </c>
+      <c r="D392" t="s">
+        <v>12</v>
+      </c>
+      <c r="E392">
+        <v>31</v>
+      </c>
+      <c r="F392">
+        <v>0</v>
+      </c>
+      <c r="G392">
+        <v>1</v>
+      </c>
+      <c r="H392">
+        <v>1</v>
+      </c>
+      <c r="I392">
+        <v>1</v>
+      </c>
+      <c r="J392">
+        <v>1</v>
+      </c>
+      <c r="K392">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="393" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A393">
+        <v>20240813</v>
+      </c>
+      <c r="B393">
+        <v>49</v>
+      </c>
+      <c r="C393" t="s">
+        <v>16</v>
+      </c>
+      <c r="D393" t="s">
+        <v>12</v>
+      </c>
+      <c r="E393">
+        <v>32</v>
+      </c>
+      <c r="F393">
+        <v>0</v>
+      </c>
+      <c r="G393">
+        <v>0</v>
+      </c>
+      <c r="H393">
+        <v>1</v>
+      </c>
+      <c r="I393">
+        <v>1</v>
+      </c>
+      <c r="J393">
+        <v>1</v>
+      </c>
+      <c r="K393">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="394" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A394">
+        <v>20240813</v>
+      </c>
+      <c r="B394">
+        <v>49</v>
+      </c>
+      <c r="C394" t="s">
+        <v>16</v>
+      </c>
+      <c r="D394" t="s">
+        <v>12</v>
+      </c>
+      <c r="E394">
+        <v>33</v>
+      </c>
+      <c r="F394">
+        <v>0</v>
+      </c>
+      <c r="G394">
+        <v>0</v>
+      </c>
+      <c r="H394">
+        <v>0</v>
+      </c>
+      <c r="I394">
+        <v>0</v>
+      </c>
+      <c r="J394">
+        <v>0</v>
+      </c>
+      <c r="K394">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="395" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A395">
+        <v>20240813</v>
+      </c>
+      <c r="B395">
+        <v>49</v>
+      </c>
+      <c r="C395" t="s">
+        <v>16</v>
+      </c>
+      <c r="D395" t="s">
+        <v>12</v>
+      </c>
+      <c r="E395">
+        <v>34</v>
+      </c>
+      <c r="F395">
+        <v>0</v>
+      </c>
+      <c r="G395">
+        <v>1</v>
+      </c>
+      <c r="H395">
+        <v>1</v>
+      </c>
+      <c r="I395">
+        <v>1</v>
+      </c>
+      <c r="J395">
+        <v>1</v>
+      </c>
+      <c r="K395">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="396" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A396">
+        <v>20240813</v>
+      </c>
+      <c r="B396">
+        <v>49</v>
+      </c>
+      <c r="C396" t="s">
+        <v>16</v>
+      </c>
+      <c r="D396" t="s">
+        <v>12</v>
+      </c>
+      <c r="E396">
+        <v>35</v>
+      </c>
+      <c r="F396">
+        <v>0</v>
+      </c>
+      <c r="G396">
+        <v>0</v>
+      </c>
+      <c r="H396">
+        <v>0</v>
+      </c>
+      <c r="I396">
+        <v>0</v>
+      </c>
+      <c r="J396">
+        <v>0</v>
+      </c>
+      <c r="K396">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="397" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A397">
+        <v>20240813</v>
+      </c>
+      <c r="B397">
+        <v>49</v>
+      </c>
+      <c r="C397" t="s">
+        <v>16</v>
+      </c>
+      <c r="D397" t="s">
+        <v>12</v>
+      </c>
+      <c r="E397">
+        <v>36</v>
+      </c>
+      <c r="F397">
+        <v>0</v>
+      </c>
+      <c r="G397">
+        <v>1</v>
+      </c>
+      <c r="H397">
+        <v>1</v>
+      </c>
+      <c r="I397">
+        <v>1</v>
+      </c>
+      <c r="J397">
+        <v>1</v>
+      </c>
+      <c r="K397">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="398" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A398">
+        <v>20240813</v>
+      </c>
+      <c r="B398">
+        <v>49</v>
+      </c>
+      <c r="C398" t="s">
+        <v>16</v>
+      </c>
+      <c r="D398" t="s">
+        <v>12</v>
+      </c>
+      <c r="E398">
+        <v>37</v>
+      </c>
+      <c r="F398">
+        <v>0</v>
+      </c>
+      <c r="G398">
+        <v>0</v>
+      </c>
+      <c r="H398">
+        <v>1</v>
+      </c>
+      <c r="I398">
+        <v>1</v>
+      </c>
+      <c r="J398">
+        <v>1</v>
+      </c>
+      <c r="K398">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="399" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A399">
+        <v>20240813</v>
+      </c>
+      <c r="B399">
+        <v>49</v>
+      </c>
+      <c r="C399" t="s">
+        <v>16</v>
+      </c>
+      <c r="D399" t="s">
+        <v>12</v>
+      </c>
+      <c r="E399">
+        <v>38</v>
+      </c>
+      <c r="F399">
+        <v>0</v>
+      </c>
+      <c r="G399">
+        <v>0</v>
+      </c>
+      <c r="H399">
+        <v>0</v>
+      </c>
+      <c r="I399">
+        <v>0</v>
+      </c>
+      <c r="J399">
+        <v>0</v>
+      </c>
+      <c r="K399">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="400" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A400">
+        <v>20240813</v>
+      </c>
+      <c r="B400">
+        <v>49</v>
+      </c>
+      <c r="C400" t="s">
+        <v>16</v>
+      </c>
+      <c r="D400" t="s">
+        <v>12</v>
+      </c>
+      <c r="E400">
+        <v>39</v>
+      </c>
+      <c r="F400">
+        <v>0</v>
+      </c>
+      <c r="G400">
+        <v>0</v>
+      </c>
+      <c r="H400">
+        <v>1</v>
+      </c>
+      <c r="I400">
+        <v>1</v>
+      </c>
+      <c r="J400">
+        <v>1</v>
+      </c>
+      <c r="K400">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="401" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A401">
+        <v>20240813</v>
+      </c>
+      <c r="B401">
+        <v>49</v>
+      </c>
+      <c r="C401" t="s">
+        <v>16</v>
+      </c>
+      <c r="D401" t="s">
+        <v>12</v>
+      </c>
+      <c r="E401">
+        <v>40</v>
+      </c>
+      <c r="F401">
+        <v>0</v>
+      </c>
+      <c r="G401">
+        <v>0</v>
+      </c>
+      <c r="H401">
+        <v>1</v>
+      </c>
+      <c r="I401">
+        <v>1</v>
+      </c>
+      <c r="J401">
+        <v>1</v>
+      </c>
+      <c r="K401">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added final survival data for resazurin
</commit_message>
<xml_diff>
--- a/data/survival/survival_resazurin.xlsx
+++ b/data/survival/survival_resazurin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/10K-seed-Cgigas/data/survival/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474F4954-B4C6-4F41-910B-C164FD376379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEAF813F-C96C-3C40-B4B1-9A0BC1F6FD76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-620" yWindow="760" windowWidth="18160" windowHeight="17720" xr2:uid="{FF76C7E6-3408-934E-9F62-D1FDE39EF6F8}"/>
+    <workbookView xWindow="-21080" yWindow="-1460" windowWidth="18160" windowHeight="17720" xr2:uid="{FF76C7E6-3408-934E-9F62-D1FDE39EF6F8}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="17">
   <si>
     <t>date.resazurin</t>
   </si>
@@ -459,11 +459,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE0A6E7-C44F-C349-A3CE-3BF585EE18ED}">
-  <dimension ref="A1:K401"/>
+  <dimension ref="A1:K441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A367" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K401" sqref="K401"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A414" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L435" sqref="L435"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14505,6 +14505,1406 @@
         <v>1</v>
       </c>
       <c r="K401">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="402" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A402">
+        <v>20240815</v>
+      </c>
+      <c r="B402">
+        <v>76</v>
+      </c>
+      <c r="C402" t="s">
+        <v>15</v>
+      </c>
+      <c r="D402" t="s">
+        <v>11</v>
+      </c>
+      <c r="E402">
+        <v>1</v>
+      </c>
+      <c r="F402">
+        <v>0</v>
+      </c>
+      <c r="G402">
+        <v>0</v>
+      </c>
+      <c r="H402">
+        <v>0</v>
+      </c>
+      <c r="I402">
+        <v>0</v>
+      </c>
+      <c r="J402">
+        <v>0</v>
+      </c>
+      <c r="K402">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="403" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A403">
+        <v>20240815</v>
+      </c>
+      <c r="B403">
+        <v>76</v>
+      </c>
+      <c r="C403" t="s">
+        <v>15</v>
+      </c>
+      <c r="D403" t="s">
+        <v>11</v>
+      </c>
+      <c r="E403">
+        <v>2</v>
+      </c>
+      <c r="F403">
+        <v>0</v>
+      </c>
+      <c r="G403">
+        <v>0</v>
+      </c>
+      <c r="H403">
+        <v>0</v>
+      </c>
+      <c r="I403">
+        <v>0</v>
+      </c>
+      <c r="J403">
+        <v>0</v>
+      </c>
+      <c r="K403">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="404" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A404">
+        <v>20240815</v>
+      </c>
+      <c r="B404">
+        <v>76</v>
+      </c>
+      <c r="C404" t="s">
+        <v>15</v>
+      </c>
+      <c r="D404" t="s">
+        <v>11</v>
+      </c>
+      <c r="E404">
+        <v>3</v>
+      </c>
+      <c r="F404">
+        <v>0</v>
+      </c>
+      <c r="G404">
+        <v>0</v>
+      </c>
+      <c r="H404">
+        <v>0</v>
+      </c>
+      <c r="I404">
+        <v>0</v>
+      </c>
+      <c r="J404">
+        <v>0</v>
+      </c>
+      <c r="K404">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="405" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A405">
+        <v>20240815</v>
+      </c>
+      <c r="B405">
+        <v>76</v>
+      </c>
+      <c r="C405" t="s">
+        <v>15</v>
+      </c>
+      <c r="D405" t="s">
+        <v>11</v>
+      </c>
+      <c r="E405">
+        <v>4</v>
+      </c>
+      <c r="F405">
+        <v>0</v>
+      </c>
+      <c r="G405">
+        <v>0</v>
+      </c>
+      <c r="H405">
+        <v>0</v>
+      </c>
+      <c r="I405">
+        <v>0</v>
+      </c>
+      <c r="J405">
+        <v>0</v>
+      </c>
+      <c r="K405">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="406" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A406">
+        <v>20240815</v>
+      </c>
+      <c r="B406">
+        <v>76</v>
+      </c>
+      <c r="C406" t="s">
+        <v>15</v>
+      </c>
+      <c r="D406" t="s">
+        <v>11</v>
+      </c>
+      <c r="E406">
+        <v>5</v>
+      </c>
+      <c r="F406">
+        <v>0</v>
+      </c>
+      <c r="G406">
+        <v>0</v>
+      </c>
+      <c r="H406">
+        <v>0</v>
+      </c>
+      <c r="I406">
+        <v>0</v>
+      </c>
+      <c r="J406">
+        <v>0</v>
+      </c>
+      <c r="K406">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="407" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A407">
+        <v>20240815</v>
+      </c>
+      <c r="B407">
+        <v>76</v>
+      </c>
+      <c r="C407" t="s">
+        <v>15</v>
+      </c>
+      <c r="D407" t="s">
+        <v>11</v>
+      </c>
+      <c r="E407">
+        <v>6</v>
+      </c>
+      <c r="F407">
+        <v>0</v>
+      </c>
+      <c r="G407">
+        <v>0</v>
+      </c>
+      <c r="H407">
+        <v>0</v>
+      </c>
+      <c r="I407">
+        <v>0</v>
+      </c>
+      <c r="J407">
+        <v>0</v>
+      </c>
+      <c r="K407">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="408" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A408">
+        <v>20240815</v>
+      </c>
+      <c r="B408">
+        <v>76</v>
+      </c>
+      <c r="C408" t="s">
+        <v>15</v>
+      </c>
+      <c r="D408" t="s">
+        <v>11</v>
+      </c>
+      <c r="E408">
+        <v>7</v>
+      </c>
+      <c r="F408">
+        <v>0</v>
+      </c>
+      <c r="G408">
+        <v>0</v>
+      </c>
+      <c r="H408">
+        <v>0</v>
+      </c>
+      <c r="I408">
+        <v>0</v>
+      </c>
+      <c r="J408">
+        <v>0</v>
+      </c>
+      <c r="K408">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="409" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A409">
+        <v>20240815</v>
+      </c>
+      <c r="B409">
+        <v>76</v>
+      </c>
+      <c r="C409" t="s">
+        <v>15</v>
+      </c>
+      <c r="D409" t="s">
+        <v>11</v>
+      </c>
+      <c r="E409">
+        <v>8</v>
+      </c>
+      <c r="F409">
+        <v>0</v>
+      </c>
+      <c r="G409">
+        <v>0</v>
+      </c>
+      <c r="H409">
+        <v>0</v>
+      </c>
+      <c r="I409">
+        <v>0</v>
+      </c>
+      <c r="J409">
+        <v>0</v>
+      </c>
+      <c r="K409">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="410" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A410">
+        <v>20240815</v>
+      </c>
+      <c r="B410">
+        <v>76</v>
+      </c>
+      <c r="C410" t="s">
+        <v>15</v>
+      </c>
+      <c r="D410" t="s">
+        <v>11</v>
+      </c>
+      <c r="E410">
+        <v>9</v>
+      </c>
+      <c r="F410">
+        <v>0</v>
+      </c>
+      <c r="G410">
+        <v>0</v>
+      </c>
+      <c r="H410">
+        <v>0</v>
+      </c>
+      <c r="I410">
+        <v>0</v>
+      </c>
+      <c r="J410">
+        <v>0</v>
+      </c>
+      <c r="K410">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="411" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A411">
+        <v>20240815</v>
+      </c>
+      <c r="B411">
+        <v>76</v>
+      </c>
+      <c r="C411" t="s">
+        <v>15</v>
+      </c>
+      <c r="D411" t="s">
+        <v>11</v>
+      </c>
+      <c r="E411">
+        <v>10</v>
+      </c>
+      <c r="F411">
+        <v>0</v>
+      </c>
+      <c r="G411">
+        <v>0</v>
+      </c>
+      <c r="H411">
+        <v>0</v>
+      </c>
+      <c r="I411">
+        <v>0</v>
+      </c>
+      <c r="J411">
+        <v>1</v>
+      </c>
+      <c r="K411">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="412" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A412">
+        <v>20240815</v>
+      </c>
+      <c r="B412">
+        <v>76</v>
+      </c>
+      <c r="C412" t="s">
+        <v>15</v>
+      </c>
+      <c r="D412" t="s">
+        <v>11</v>
+      </c>
+      <c r="E412">
+        <v>11</v>
+      </c>
+      <c r="F412">
+        <v>0</v>
+      </c>
+      <c r="G412">
+        <v>0</v>
+      </c>
+      <c r="H412">
+        <v>0</v>
+      </c>
+      <c r="I412">
+        <v>0</v>
+      </c>
+      <c r="J412">
+        <v>0</v>
+      </c>
+      <c r="K412">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="413" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A413">
+        <v>20240815</v>
+      </c>
+      <c r="B413">
+        <v>76</v>
+      </c>
+      <c r="C413" t="s">
+        <v>15</v>
+      </c>
+      <c r="D413" t="s">
+        <v>11</v>
+      </c>
+      <c r="E413">
+        <v>12</v>
+      </c>
+      <c r="F413">
+        <v>0</v>
+      </c>
+      <c r="G413">
+        <v>0</v>
+      </c>
+      <c r="H413">
+        <v>0</v>
+      </c>
+      <c r="I413">
+        <v>0</v>
+      </c>
+      <c r="J413">
+        <v>0</v>
+      </c>
+      <c r="K413">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="414" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A414">
+        <v>20240815</v>
+      </c>
+      <c r="B414">
+        <v>76</v>
+      </c>
+      <c r="C414" t="s">
+        <v>15</v>
+      </c>
+      <c r="D414" t="s">
+        <v>11</v>
+      </c>
+      <c r="E414">
+        <v>13</v>
+      </c>
+      <c r="F414">
+        <v>0</v>
+      </c>
+      <c r="G414">
+        <v>0</v>
+      </c>
+      <c r="H414">
+        <v>0</v>
+      </c>
+      <c r="I414">
+        <v>0</v>
+      </c>
+      <c r="J414">
+        <v>0</v>
+      </c>
+      <c r="K414">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="415" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A415">
+        <v>20240815</v>
+      </c>
+      <c r="B415">
+        <v>76</v>
+      </c>
+      <c r="C415" t="s">
+        <v>15</v>
+      </c>
+      <c r="D415" t="s">
+        <v>11</v>
+      </c>
+      <c r="E415">
+        <v>14</v>
+      </c>
+      <c r="F415">
+        <v>0</v>
+      </c>
+      <c r="G415">
+        <v>0</v>
+      </c>
+      <c r="H415">
+        <v>0</v>
+      </c>
+      <c r="I415">
+        <v>0</v>
+      </c>
+      <c r="J415">
+        <v>0</v>
+      </c>
+      <c r="K415">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="416" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A416">
+        <v>20240815</v>
+      </c>
+      <c r="B416">
+        <v>76</v>
+      </c>
+      <c r="C416" t="s">
+        <v>15</v>
+      </c>
+      <c r="D416" t="s">
+        <v>11</v>
+      </c>
+      <c r="E416">
+        <v>15</v>
+      </c>
+      <c r="F416">
+        <v>0</v>
+      </c>
+      <c r="G416">
+        <v>0</v>
+      </c>
+      <c r="H416">
+        <v>0</v>
+      </c>
+      <c r="I416">
+        <v>0</v>
+      </c>
+      <c r="J416">
+        <v>0</v>
+      </c>
+      <c r="K416">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="417" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A417">
+        <v>20240815</v>
+      </c>
+      <c r="B417">
+        <v>76</v>
+      </c>
+      <c r="C417" t="s">
+        <v>15</v>
+      </c>
+      <c r="D417" t="s">
+        <v>11</v>
+      </c>
+      <c r="E417">
+        <v>16</v>
+      </c>
+      <c r="F417">
+        <v>0</v>
+      </c>
+      <c r="G417">
+        <v>0</v>
+      </c>
+      <c r="H417">
+        <v>0</v>
+      </c>
+      <c r="I417">
+        <v>0</v>
+      </c>
+      <c r="J417">
+        <v>0</v>
+      </c>
+      <c r="K417">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="418" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A418">
+        <v>20240815</v>
+      </c>
+      <c r="B418">
+        <v>76</v>
+      </c>
+      <c r="C418" t="s">
+        <v>15</v>
+      </c>
+      <c r="D418" t="s">
+        <v>11</v>
+      </c>
+      <c r="E418">
+        <v>17</v>
+      </c>
+      <c r="F418">
+        <v>0</v>
+      </c>
+      <c r="G418">
+        <v>0</v>
+      </c>
+      <c r="H418">
+        <v>0</v>
+      </c>
+      <c r="I418">
+        <v>0</v>
+      </c>
+      <c r="J418">
+        <v>0</v>
+      </c>
+      <c r="K418">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="419" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A419">
+        <v>20240815</v>
+      </c>
+      <c r="B419">
+        <v>76</v>
+      </c>
+      <c r="C419" t="s">
+        <v>15</v>
+      </c>
+      <c r="D419" t="s">
+        <v>11</v>
+      </c>
+      <c r="E419">
+        <v>18</v>
+      </c>
+      <c r="F419">
+        <v>0</v>
+      </c>
+      <c r="G419">
+        <v>0</v>
+      </c>
+      <c r="H419">
+        <v>0</v>
+      </c>
+      <c r="I419">
+        <v>0</v>
+      </c>
+      <c r="J419">
+        <v>0</v>
+      </c>
+      <c r="K419">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="420" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A420">
+        <v>20240815</v>
+      </c>
+      <c r="B420">
+        <v>76</v>
+      </c>
+      <c r="C420" t="s">
+        <v>15</v>
+      </c>
+      <c r="D420" t="s">
+        <v>11</v>
+      </c>
+      <c r="E420">
+        <v>19</v>
+      </c>
+      <c r="F420">
+        <v>0</v>
+      </c>
+      <c r="G420">
+        <v>0</v>
+      </c>
+      <c r="H420">
+        <v>0</v>
+      </c>
+      <c r="I420">
+        <v>0</v>
+      </c>
+      <c r="J420">
+        <v>0</v>
+      </c>
+      <c r="K420">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="421" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A421">
+        <v>20240815</v>
+      </c>
+      <c r="B421">
+        <v>76</v>
+      </c>
+      <c r="C421" t="s">
+        <v>15</v>
+      </c>
+      <c r="D421" t="s">
+        <v>11</v>
+      </c>
+      <c r="E421">
+        <v>20</v>
+      </c>
+      <c r="F421">
+        <v>0</v>
+      </c>
+      <c r="G421">
+        <v>0</v>
+      </c>
+      <c r="H421">
+        <v>0</v>
+      </c>
+      <c r="I421">
+        <v>0</v>
+      </c>
+      <c r="J421">
+        <v>0</v>
+      </c>
+      <c r="K421">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="422" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A422">
+        <v>20240815</v>
+      </c>
+      <c r="B422">
+        <v>76</v>
+      </c>
+      <c r="C422" t="s">
+        <v>15</v>
+      </c>
+      <c r="D422" t="s">
+        <v>12</v>
+      </c>
+      <c r="E422">
+        <v>21</v>
+      </c>
+      <c r="F422">
+        <v>0</v>
+      </c>
+      <c r="G422">
+        <v>0</v>
+      </c>
+      <c r="H422">
+        <v>1</v>
+      </c>
+      <c r="I422">
+        <v>1</v>
+      </c>
+      <c r="J422">
+        <v>1</v>
+      </c>
+      <c r="K422">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="423" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A423">
+        <v>20240815</v>
+      </c>
+      <c r="B423">
+        <v>76</v>
+      </c>
+      <c r="C423" t="s">
+        <v>15</v>
+      </c>
+      <c r="D423" t="s">
+        <v>12</v>
+      </c>
+      <c r="E423">
+        <v>22</v>
+      </c>
+      <c r="F423">
+        <v>0</v>
+      </c>
+      <c r="G423">
+        <v>0</v>
+      </c>
+      <c r="H423">
+        <v>1</v>
+      </c>
+      <c r="I423">
+        <v>1</v>
+      </c>
+      <c r="J423">
+        <v>1</v>
+      </c>
+      <c r="K423">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="424" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A424">
+        <v>20240815</v>
+      </c>
+      <c r="B424">
+        <v>76</v>
+      </c>
+      <c r="C424" t="s">
+        <v>15</v>
+      </c>
+      <c r="D424" t="s">
+        <v>12</v>
+      </c>
+      <c r="E424">
+        <v>23</v>
+      </c>
+      <c r="F424">
+        <v>0</v>
+      </c>
+      <c r="G424">
+        <v>0</v>
+      </c>
+      <c r="H424">
+        <v>0</v>
+      </c>
+      <c r="I424">
+        <v>0</v>
+      </c>
+      <c r="J424">
+        <v>0</v>
+      </c>
+      <c r="K424">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="425" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A425">
+        <v>20240815</v>
+      </c>
+      <c r="B425">
+        <v>76</v>
+      </c>
+      <c r="C425" t="s">
+        <v>15</v>
+      </c>
+      <c r="D425" t="s">
+        <v>12</v>
+      </c>
+      <c r="E425">
+        <v>24</v>
+      </c>
+      <c r="F425">
+        <v>0</v>
+      </c>
+      <c r="G425">
+        <v>0</v>
+      </c>
+      <c r="H425">
+        <v>0</v>
+      </c>
+      <c r="I425">
+        <v>0</v>
+      </c>
+      <c r="J425">
+        <v>0</v>
+      </c>
+      <c r="K425">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="426" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A426">
+        <v>20240815</v>
+      </c>
+      <c r="B426">
+        <v>76</v>
+      </c>
+      <c r="C426" t="s">
+        <v>15</v>
+      </c>
+      <c r="D426" t="s">
+        <v>12</v>
+      </c>
+      <c r="E426">
+        <v>25</v>
+      </c>
+      <c r="F426">
+        <v>0</v>
+      </c>
+      <c r="G426">
+        <v>0</v>
+      </c>
+      <c r="H426">
+        <v>0</v>
+      </c>
+      <c r="I426">
+        <v>0</v>
+      </c>
+      <c r="J426">
+        <v>0</v>
+      </c>
+      <c r="K426">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="427" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A427">
+        <v>20240815</v>
+      </c>
+      <c r="B427">
+        <v>76</v>
+      </c>
+      <c r="C427" t="s">
+        <v>15</v>
+      </c>
+      <c r="D427" t="s">
+        <v>12</v>
+      </c>
+      <c r="E427">
+        <v>26</v>
+      </c>
+      <c r="F427">
+        <v>0</v>
+      </c>
+      <c r="G427">
+        <v>0</v>
+      </c>
+      <c r="H427">
+        <v>1</v>
+      </c>
+      <c r="I427">
+        <v>1</v>
+      </c>
+      <c r="J427">
+        <v>1</v>
+      </c>
+      <c r="K427">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="428" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A428">
+        <v>20240815</v>
+      </c>
+      <c r="B428">
+        <v>76</v>
+      </c>
+      <c r="C428" t="s">
+        <v>15</v>
+      </c>
+      <c r="D428" t="s">
+        <v>12</v>
+      </c>
+      <c r="E428">
+        <v>27</v>
+      </c>
+      <c r="F428">
+        <v>0</v>
+      </c>
+      <c r="G428">
+        <v>0</v>
+      </c>
+      <c r="H428">
+        <v>0</v>
+      </c>
+      <c r="I428">
+        <v>0</v>
+      </c>
+      <c r="J428">
+        <v>0</v>
+      </c>
+      <c r="K428">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="429" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A429">
+        <v>20240815</v>
+      </c>
+      <c r="B429">
+        <v>76</v>
+      </c>
+      <c r="C429" t="s">
+        <v>15</v>
+      </c>
+      <c r="D429" t="s">
+        <v>12</v>
+      </c>
+      <c r="E429">
+        <v>28</v>
+      </c>
+      <c r="F429">
+        <v>0</v>
+      </c>
+      <c r="G429">
+        <v>0</v>
+      </c>
+      <c r="H429">
+        <v>0</v>
+      </c>
+      <c r="I429">
+        <v>1</v>
+      </c>
+      <c r="J429">
+        <v>1</v>
+      </c>
+      <c r="K429">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="430" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A430">
+        <v>20240815</v>
+      </c>
+      <c r="B430">
+        <v>76</v>
+      </c>
+      <c r="C430" t="s">
+        <v>15</v>
+      </c>
+      <c r="D430" t="s">
+        <v>12</v>
+      </c>
+      <c r="E430">
+        <v>29</v>
+      </c>
+      <c r="F430">
+        <v>0</v>
+      </c>
+      <c r="G430">
+        <v>0</v>
+      </c>
+      <c r="H430">
+        <v>0</v>
+      </c>
+      <c r="I430">
+        <v>0</v>
+      </c>
+      <c r="J430">
+        <v>0</v>
+      </c>
+      <c r="K430">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="431" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A431">
+        <v>20240815</v>
+      </c>
+      <c r="B431">
+        <v>76</v>
+      </c>
+      <c r="C431" t="s">
+        <v>15</v>
+      </c>
+      <c r="D431" t="s">
+        <v>12</v>
+      </c>
+      <c r="E431">
+        <v>30</v>
+      </c>
+      <c r="F431">
+        <v>0</v>
+      </c>
+      <c r="G431">
+        <v>0</v>
+      </c>
+      <c r="H431">
+        <v>0</v>
+      </c>
+      <c r="I431">
+        <v>0</v>
+      </c>
+      <c r="J431">
+        <v>0</v>
+      </c>
+      <c r="K431">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="432" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A432">
+        <v>20240815</v>
+      </c>
+      <c r="B432">
+        <v>76</v>
+      </c>
+      <c r="C432" t="s">
+        <v>15</v>
+      </c>
+      <c r="D432" t="s">
+        <v>12</v>
+      </c>
+      <c r="E432">
+        <v>31</v>
+      </c>
+      <c r="F432">
+        <v>0</v>
+      </c>
+      <c r="G432">
+        <v>0</v>
+      </c>
+      <c r="H432">
+        <v>1</v>
+      </c>
+      <c r="I432">
+        <v>1</v>
+      </c>
+      <c r="J432">
+        <v>1</v>
+      </c>
+      <c r="K432">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="433" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A433">
+        <v>20240815</v>
+      </c>
+      <c r="B433">
+        <v>76</v>
+      </c>
+      <c r="C433" t="s">
+        <v>15</v>
+      </c>
+      <c r="D433" t="s">
+        <v>12</v>
+      </c>
+      <c r="E433">
+        <v>32</v>
+      </c>
+      <c r="F433">
+        <v>0</v>
+      </c>
+      <c r="G433">
+        <v>0</v>
+      </c>
+      <c r="H433">
+        <v>1</v>
+      </c>
+      <c r="I433">
+        <v>1</v>
+      </c>
+      <c r="J433">
+        <v>1</v>
+      </c>
+      <c r="K433">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="434" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A434">
+        <v>20240815</v>
+      </c>
+      <c r="B434">
+        <v>76</v>
+      </c>
+      <c r="C434" t="s">
+        <v>15</v>
+      </c>
+      <c r="D434" t="s">
+        <v>12</v>
+      </c>
+      <c r="E434">
+        <v>33</v>
+      </c>
+      <c r="F434">
+        <v>0</v>
+      </c>
+      <c r="G434">
+        <v>0</v>
+      </c>
+      <c r="H434">
+        <v>0</v>
+      </c>
+      <c r="I434">
+        <v>0</v>
+      </c>
+      <c r="J434">
+        <v>0</v>
+      </c>
+      <c r="K434">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="435" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A435">
+        <v>20240815</v>
+      </c>
+      <c r="B435">
+        <v>76</v>
+      </c>
+      <c r="C435" t="s">
+        <v>15</v>
+      </c>
+      <c r="D435" t="s">
+        <v>12</v>
+      </c>
+      <c r="E435">
+        <v>34</v>
+      </c>
+      <c r="F435">
+        <v>0</v>
+      </c>
+      <c r="G435">
+        <v>0</v>
+      </c>
+      <c r="H435">
+        <v>1</v>
+      </c>
+      <c r="I435">
+        <v>1</v>
+      </c>
+      <c r="J435">
+        <v>1</v>
+      </c>
+      <c r="K435">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="436" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A436">
+        <v>20240815</v>
+      </c>
+      <c r="B436">
+        <v>76</v>
+      </c>
+      <c r="C436" t="s">
+        <v>15</v>
+      </c>
+      <c r="D436" t="s">
+        <v>12</v>
+      </c>
+      <c r="E436">
+        <v>35</v>
+      </c>
+      <c r="F436">
+        <v>0</v>
+      </c>
+      <c r="G436">
+        <v>0</v>
+      </c>
+      <c r="H436">
+        <v>0</v>
+      </c>
+      <c r="I436">
+        <v>0</v>
+      </c>
+      <c r="J436">
+        <v>1</v>
+      </c>
+      <c r="K436">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="437" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A437">
+        <v>20240815</v>
+      </c>
+      <c r="B437">
+        <v>76</v>
+      </c>
+      <c r="C437" t="s">
+        <v>15</v>
+      </c>
+      <c r="D437" t="s">
+        <v>12</v>
+      </c>
+      <c r="E437">
+        <v>36</v>
+      </c>
+      <c r="F437">
+        <v>0</v>
+      </c>
+      <c r="G437">
+        <v>0</v>
+      </c>
+      <c r="H437">
+        <v>0</v>
+      </c>
+      <c r="I437">
+        <v>0</v>
+      </c>
+      <c r="J437">
+        <v>0</v>
+      </c>
+      <c r="K437">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="438" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A438">
+        <v>20240815</v>
+      </c>
+      <c r="B438">
+        <v>76</v>
+      </c>
+      <c r="C438" t="s">
+        <v>15</v>
+      </c>
+      <c r="D438" t="s">
+        <v>12</v>
+      </c>
+      <c r="E438">
+        <v>37</v>
+      </c>
+      <c r="F438">
+        <v>0</v>
+      </c>
+      <c r="G438">
+        <v>0</v>
+      </c>
+      <c r="H438">
+        <v>1</v>
+      </c>
+      <c r="I438">
+        <v>1</v>
+      </c>
+      <c r="J438">
+        <v>1</v>
+      </c>
+      <c r="K438">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="439" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A439">
+        <v>20240815</v>
+      </c>
+      <c r="B439">
+        <v>76</v>
+      </c>
+      <c r="C439" t="s">
+        <v>15</v>
+      </c>
+      <c r="D439" t="s">
+        <v>12</v>
+      </c>
+      <c r="E439">
+        <v>38</v>
+      </c>
+      <c r="F439">
+        <v>0</v>
+      </c>
+      <c r="G439">
+        <v>0</v>
+      </c>
+      <c r="H439">
+        <v>1</v>
+      </c>
+      <c r="I439">
+        <v>1</v>
+      </c>
+      <c r="J439">
+        <v>1</v>
+      </c>
+      <c r="K439">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="440" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A440">
+        <v>20240815</v>
+      </c>
+      <c r="B440">
+        <v>76</v>
+      </c>
+      <c r="C440" t="s">
+        <v>15</v>
+      </c>
+      <c r="D440" t="s">
+        <v>12</v>
+      </c>
+      <c r="E440">
+        <v>39</v>
+      </c>
+      <c r="F440">
+        <v>0</v>
+      </c>
+      <c r="G440">
+        <v>0</v>
+      </c>
+      <c r="H440">
+        <v>1</v>
+      </c>
+      <c r="I440">
+        <v>1</v>
+      </c>
+      <c r="J440">
+        <v>1</v>
+      </c>
+      <c r="K440">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="441" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A441">
+        <v>20240815</v>
+      </c>
+      <c r="B441">
+        <v>76</v>
+      </c>
+      <c r="C441" t="s">
+        <v>15</v>
+      </c>
+      <c r="D441" t="s">
+        <v>12</v>
+      </c>
+      <c r="E441">
+        <v>40</v>
+      </c>
+      <c r="F441">
+        <v>0</v>
+      </c>
+      <c r="G441">
+        <v>0</v>
+      </c>
+      <c r="H441">
+        <v>0</v>
+      </c>
+      <c r="I441">
+        <v>0</v>
+      </c>
+      <c r="J441">
+        <v>0</v>
+      </c>
+      <c r="K441">
         <v>1</v>
       </c>
     </row>

</xml_diff>